<commit_message>
Updated docs to reflect "SplitCategory" field
</commit_message>
<xml_diff>
--- a/GazetteerETL/Resources/UniversalGazetterModel.xlsx
+++ b/GazetteerETL/Resources/UniversalGazetterModel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7616" uniqueCount="4293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7620" uniqueCount="4296">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -12906,6 +12906,15 @@
   </si>
   <si>
     <t>A category used to indicate the category/type of name: natural language,code, abbreviated name, phonetic …. The vast majority of the gazetteer will have the vale NAME. meaning a natural language name for a place</t>
+  </si>
+  <si>
+    <t>Splitcategory</t>
+  </si>
+  <si>
+    <t>range:[NonLatin,Rare,Basic,WellKnown,&lt;BLANK&gt;]</t>
+  </si>
+  <si>
+    <t>This field indicates a broad category to which the record belongs intended to be used to partition the gazetteer to allow subsets  of the gazetteer to be used while still covering most of the commonly mentioned places. Basic plus WellKnow for a small but well performing subset.</t>
   </si>
 </sst>
 </file>
@@ -13778,10 +13787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14107,6 +14116,20 @@
       </c>
       <c r="D25" t="s">
         <v>4290</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4293</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4283</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4294</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First cut at Gazetteer 2.0
Solr config moved to other projects, build.xml cleaned up,  ETL set to
use new looser deduping ,and docs edited to match changes
</commit_message>
<xml_diff>
--- a/GazetteerETL/Resources/UniversalGazetterModel.xlsx
+++ b/GazetteerETL/Resources/UniversalGazetterModel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-1365" yWindow="-165" windowWidth="25320" windowHeight="14535"/>
+    <workbookView xWindow="-1365" yWindow="-165" windowWidth="25320" windowHeight="14535" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PLACE_NAMES" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Country_Code!$A$1:$J$283</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Country_Code FIPS to ISO'!$A$1:$J$283</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FEATURE_CLASS!$A$1:$B$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FEATURE_CODE!$A$1:$G$704</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FEATURE_CODE!$A$1:$G$705</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PLACE_NAMES!$A$2:$D$21</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">Country_Code!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Country_Code FIPS to ISO'!$1:$1</definedName>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7620" uniqueCount="4296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7621" uniqueCount="4297">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -12908,13 +12908,16 @@
     <t>A category used to indicate the category/type of name: natural language,code, abbreviated name, phonetic …. The vast majority of the gazetteer will have the vale NAME. meaning a natural language name for a place</t>
   </si>
   <si>
-    <t>Splitcategory</t>
-  </si>
-  <si>
-    <t>range:[NonLatin,Rare,Basic,WellKnown,&lt;BLANK&gt;]</t>
-  </si>
-  <si>
-    <t>This field indicates a broad category to which the record belongs intended to be used to partition the gazetteer to allow subsets  of the gazetteer to be used while still covering most of the commonly mentioned places. Basic plus WellKnow for a small but well performing subset.</t>
+    <t>RSTNH</t>
+  </si>
+  <si>
+    <t>historical railroad station</t>
+  </si>
+  <si>
+    <t>a former facility comprising ticket office, platforms, etc. for loading and unloading train passengers and freight</t>
+  </si>
+  <si>
+    <t>S-RSTNH</t>
   </si>
 </sst>
 </file>
@@ -13787,10 +13790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14116,20 +14119,6 @@
       </c>
       <c r="D25" t="s">
         <v>4290</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>4293</v>
-      </c>
-      <c r="B26" t="s">
-        <v>4283</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4294</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4295</v>
       </c>
     </row>
   </sheetData>
@@ -14242,17 +14231,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G704"/>
+  <dimension ref="A1:G705"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A708" sqref="A708"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" style="12" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.28515625" style="12" bestFit="1" customWidth="1"/>
@@ -26535,16 +26524,19 @@
     </row>
     <row r="541" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A541" s="12" t="s">
-        <v>295</v>
+        <v>4293</v>
       </c>
       <c r="B541" s="12" t="s">
-        <v>722</v>
+        <v>4294</v>
+      </c>
+      <c r="C541" s="12" t="s">
+        <v>4295</v>
       </c>
       <c r="D541" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E541" s="12" t="s">
-        <v>3980</v>
+        <v>4296</v>
       </c>
       <c r="F541" s="12">
         <v>0</v>
@@ -26555,19 +26547,16 @@
     </row>
     <row r="542" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A542" s="12" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="B542" s="12" t="s">
-        <v>723</v>
-      </c>
-      <c r="C542" s="12" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D542" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E542" s="12" t="s">
-        <v>3981</v>
+        <v>3980</v>
       </c>
       <c r="F542" s="12">
         <v>0</v>
@@ -26578,16 +26567,19 @@
     </row>
     <row r="543" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A543" s="12" t="s">
-        <v>584</v>
+        <v>284</v>
       </c>
       <c r="B543" s="12" t="s">
-        <v>725</v>
+        <v>723</v>
+      </c>
+      <c r="C543" s="12" t="s">
+        <v>724</v>
       </c>
       <c r="D543" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E543" s="12" t="s">
-        <v>3982</v>
+        <v>3981</v>
       </c>
       <c r="F543" s="12">
         <v>0</v>
@@ -26598,19 +26590,16 @@
     </row>
     <row r="544" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A544" s="12" t="s">
-        <v>101</v>
+        <v>584</v>
       </c>
       <c r="B544" s="12" t="s">
-        <v>726</v>
-      </c>
-      <c r="C544" s="12" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D544" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E544" s="12" t="s">
-        <v>3983</v>
+        <v>3982</v>
       </c>
       <c r="F544" s="12">
         <v>0</v>
@@ -26621,16 +26610,19 @@
     </row>
     <row r="545" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A545" s="12" t="s">
-        <v>514</v>
+        <v>101</v>
       </c>
       <c r="B545" s="12" t="s">
-        <v>728</v>
+        <v>726</v>
+      </c>
+      <c r="C545" s="12" t="s">
+        <v>727</v>
       </c>
       <c r="D545" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E545" s="12" t="s">
-        <v>3984</v>
+        <v>3983</v>
       </c>
       <c r="F545" s="12">
         <v>0</v>
@@ -26641,19 +26633,16 @@
     </row>
     <row r="546" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A546" s="12" t="s">
-        <v>199</v>
+        <v>514</v>
       </c>
       <c r="B546" s="12" t="s">
-        <v>729</v>
-      </c>
-      <c r="C546" s="12" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D546" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E546" s="12" t="s">
-        <v>3985</v>
+        <v>3984</v>
       </c>
       <c r="F546" s="12">
         <v>0</v>
@@ -26664,19 +26653,19 @@
     </row>
     <row r="547" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A547" s="12" t="s">
-        <v>252</v>
+        <v>199</v>
       </c>
       <c r="B547" s="12" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C547" s="12" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D547" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E547" s="12" t="s">
-        <v>3986</v>
+        <v>3985</v>
       </c>
       <c r="F547" s="12">
         <v>0</v>
@@ -26687,19 +26676,19 @@
     </row>
     <row r="548" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A548" s="12" t="s">
-        <v>115</v>
+        <v>252</v>
       </c>
       <c r="B548" s="12" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C548" s="12" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D548" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E548" s="12" t="s">
-        <v>3987</v>
+        <v>3986</v>
       </c>
       <c r="F548" s="12">
         <v>0</v>
@@ -26710,19 +26699,19 @@
     </row>
     <row r="549" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A549" s="12" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B549" s="12" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C549" s="12" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D549" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E549" s="12" t="s">
-        <v>3988</v>
+        <v>3987</v>
       </c>
       <c r="F549" s="12">
         <v>0</v>
@@ -26733,19 +26722,19 @@
     </row>
     <row r="550" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A550" s="12" t="s">
-        <v>417</v>
+        <v>165</v>
       </c>
       <c r="B550" s="12" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C550" s="12" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D550" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E550" s="12" t="s">
-        <v>3989</v>
+        <v>3988</v>
       </c>
       <c r="F550" s="12">
         <v>0</v>
@@ -26756,19 +26745,19 @@
     </row>
     <row r="551" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A551" s="12" t="s">
-        <v>132</v>
+        <v>417</v>
       </c>
       <c r="B551" s="12" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C551" s="12" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D551" s="12" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E551" s="12" t="s">
-        <v>3990</v>
+        <v>3989</v>
       </c>
       <c r="F551" s="12">
         <v>0</v>
@@ -26779,19 +26768,19 @@
     </row>
     <row r="552" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A552" s="12" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="B552" s="12" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C552" s="12" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="D552" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E552" s="12" t="s">
-        <v>3991</v>
+        <v>3990</v>
       </c>
       <c r="F552" s="12">
         <v>0</v>
@@ -26802,19 +26791,19 @@
     </row>
     <row r="553" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A553" s="12" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="B553" s="12" t="s">
-        <v>983</v>
+        <v>741</v>
       </c>
       <c r="C553" s="12" t="s">
-        <v>984</v>
+        <v>742</v>
       </c>
       <c r="D553" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E553" s="12" t="s">
-        <v>3992</v>
+        <v>3991</v>
       </c>
       <c r="F553" s="12">
         <v>0</v>
@@ -26825,19 +26814,19 @@
     </row>
     <row r="554" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A554" s="12" t="s">
-        <v>122</v>
+        <v>211</v>
       </c>
       <c r="B554" s="12" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="C554" s="12" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="D554" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E554" s="12" t="s">
-        <v>3993</v>
+        <v>3992</v>
       </c>
       <c r="F554" s="12">
         <v>0</v>
@@ -26848,19 +26837,19 @@
     </row>
     <row r="555" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A555" s="12" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="B555" s="12" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="C555" s="12" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D555" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E555" s="12" t="s">
-        <v>3994</v>
+        <v>3993</v>
       </c>
       <c r="F555" s="12">
         <v>0</v>
@@ -26871,19 +26860,19 @@
     </row>
     <row r="556" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A556" s="12" t="s">
-        <v>384</v>
+        <v>170</v>
       </c>
       <c r="B556" s="12" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="C556" s="12" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="D556" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E556" s="12" t="s">
-        <v>3995</v>
+        <v>3994</v>
       </c>
       <c r="F556" s="12">
         <v>0</v>
@@ -26894,19 +26883,19 @@
     </row>
     <row r="557" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A557" s="12" t="s">
-        <v>429</v>
+        <v>384</v>
       </c>
       <c r="B557" s="12" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C557" s="12" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="D557" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E557" s="12" t="s">
-        <v>3996</v>
+        <v>3995</v>
       </c>
       <c r="F557" s="12">
         <v>0</v>
@@ -26917,19 +26906,19 @@
     </row>
     <row r="558" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A558" s="12" t="s">
-        <v>4210</v>
+        <v>429</v>
       </c>
       <c r="B558" s="12" t="s">
-        <v>4164</v>
+        <v>991</v>
       </c>
       <c r="C558" s="12" t="s">
-        <v>4165</v>
+        <v>992</v>
       </c>
       <c r="D558" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E558" s="12" t="s">
-        <v>4191</v>
+        <v>3996</v>
       </c>
       <c r="F558" s="12">
         <v>0</v>
@@ -26940,19 +26929,19 @@
     </row>
     <row r="559" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A559" s="12" t="s">
-        <v>487</v>
+        <v>4210</v>
       </c>
       <c r="B559" s="12" t="s">
-        <v>993</v>
+        <v>4164</v>
       </c>
       <c r="C559" s="12" t="s">
-        <v>994</v>
+        <v>4165</v>
       </c>
       <c r="D559" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E559" s="12" t="s">
-        <v>3997</v>
+        <v>4191</v>
       </c>
       <c r="F559" s="12">
         <v>0</v>
@@ -26963,19 +26952,19 @@
     </row>
     <row r="560" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A560" s="12" t="s">
-        <v>601</v>
+        <v>487</v>
       </c>
       <c r="B560" s="12" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C560" s="12" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="D560" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E560" s="12" t="s">
-        <v>3998</v>
+        <v>3997</v>
       </c>
       <c r="F560" s="12">
         <v>0</v>
@@ -26986,19 +26975,19 @@
     </row>
     <row r="561" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A561" s="12" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="B561" s="12" t="s">
-        <v>1286</v>
+        <v>995</v>
       </c>
       <c r="C561" s="12" t="s">
-        <v>1287</v>
+        <v>996</v>
       </c>
       <c r="D561" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E561" s="12" t="s">
-        <v>3999</v>
+        <v>3998</v>
       </c>
       <c r="F561" s="12">
         <v>0</v>
@@ -27009,19 +26998,19 @@
     </row>
     <row r="562" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A562" s="12" t="s">
-        <v>688</v>
+        <v>609</v>
       </c>
       <c r="B562" s="12" t="s">
-        <v>997</v>
+        <v>1286</v>
       </c>
       <c r="C562" s="12" t="s">
-        <v>998</v>
+        <v>1287</v>
       </c>
       <c r="D562" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E562" s="12" t="s">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="F562" s="12">
         <v>0</v>
@@ -27032,19 +27021,19 @@
     </row>
     <row r="563" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A563" s="12" t="s">
-        <v>160</v>
+        <v>688</v>
       </c>
       <c r="B563" s="12" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="C563" s="12" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D563" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E563" s="12" t="s">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="F563" s="12">
         <v>0</v>
@@ -27055,19 +27044,19 @@
     </row>
     <row r="564" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A564" s="12" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B564" s="12" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C564" s="12" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D564" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E564" s="12" t="s">
-        <v>4002</v>
+        <v>4001</v>
       </c>
       <c r="F564" s="12">
         <v>0</v>
@@ -27078,19 +27067,19 @@
     </row>
     <row r="565" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A565" s="12" t="s">
-        <v>699</v>
+        <v>155</v>
       </c>
       <c r="B565" s="12" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C565" s="12" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D565" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E565" s="12" t="s">
-        <v>4003</v>
+        <v>4002</v>
       </c>
       <c r="F565" s="12">
         <v>0</v>
@@ -27101,19 +27090,19 @@
     </row>
     <row r="566" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A566" s="12" t="s">
-        <v>389</v>
+        <v>699</v>
       </c>
       <c r="B566" s="12" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="C566" s="12" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D566" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E566" s="12" t="s">
-        <v>4004</v>
+        <v>4003</v>
       </c>
       <c r="F566" s="12">
         <v>0</v>
@@ -27124,19 +27113,19 @@
     </row>
     <row r="567" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A567" s="12" t="s">
-        <v>249</v>
+        <v>389</v>
       </c>
       <c r="B567" s="12" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="C567" s="12" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D567" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E567" s="12" t="s">
-        <v>4005</v>
+        <v>4004</v>
       </c>
       <c r="F567" s="12">
         <v>0</v>
@@ -27147,19 +27136,19 @@
     </row>
     <row r="568" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A568" s="12" t="s">
-        <v>679</v>
+        <v>249</v>
       </c>
       <c r="B568" s="12" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="C568" s="12" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D568" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E568" s="12" t="s">
-        <v>4006</v>
+        <v>4005</v>
       </c>
       <c r="F568" s="12">
         <v>0</v>
@@ -27170,65 +27159,65 @@
     </row>
     <row r="569" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A569" s="12" t="s">
-        <v>396</v>
+        <v>679</v>
       </c>
       <c r="B569" s="12" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="C569" s="12" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D569" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E569" s="12" t="s">
-        <v>4007</v>
+        <v>4006</v>
       </c>
       <c r="F569" s="12">
         <v>0</v>
       </c>
       <c r="G569" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="570" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A570" s="12" t="s">
-        <v>4211</v>
+        <v>396</v>
       </c>
       <c r="B570" s="12" t="s">
-        <v>4166</v>
+        <v>1011</v>
       </c>
       <c r="C570" s="12" t="s">
-        <v>4167</v>
+        <v>1012</v>
       </c>
       <c r="D570" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E570" s="12" t="s">
-        <v>4192</v>
+        <v>4007</v>
       </c>
       <c r="F570" s="12">
         <v>0</v>
       </c>
       <c r="G570" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="571" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A571" s="12" t="s">
-        <v>687</v>
+        <v>4211</v>
       </c>
       <c r="B571" s="12" t="s">
-        <v>1013</v>
+        <v>4166</v>
       </c>
       <c r="C571" s="12" t="s">
-        <v>1014</v>
+        <v>4167</v>
       </c>
       <c r="D571" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E571" s="12" t="s">
-        <v>4008</v>
+        <v>4192</v>
       </c>
       <c r="F571" s="12">
         <v>0</v>
@@ -27239,19 +27228,19 @@
     </row>
     <row r="572" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A572" s="12" t="s">
-        <v>603</v>
+        <v>687</v>
       </c>
       <c r="B572" s="12" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C572" s="12" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="D572" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E572" s="12" t="s">
-        <v>4009</v>
+        <v>4008</v>
       </c>
       <c r="F572" s="12">
         <v>0</v>
@@ -27262,19 +27251,19 @@
     </row>
     <row r="573" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A573" s="12" t="s">
-        <v>82</v>
+        <v>603</v>
       </c>
       <c r="B573" s="12" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C573" s="12" t="s">
         <v>1016</v>
       </c>
       <c r="D573" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E573" s="12" t="s">
-        <v>4010</v>
+        <v>4009</v>
       </c>
       <c r="F573" s="12">
         <v>0</v>
@@ -27285,19 +27274,19 @@
     </row>
     <row r="574" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A574" s="12" t="s">
-        <v>1288</v>
+        <v>82</v>
       </c>
       <c r="B574" s="12" t="s">
-        <v>1289</v>
+        <v>1017</v>
       </c>
       <c r="C574" s="12" t="s">
-        <v>1290</v>
+        <v>1016</v>
       </c>
       <c r="D574" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E574" s="12" t="s">
-        <v>4011</v>
+        <v>4010</v>
       </c>
       <c r="F574" s="12">
         <v>0</v>
@@ -27308,19 +27297,19 @@
     </row>
     <row r="575" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A575" s="12" t="s">
-        <v>545</v>
+        <v>1288</v>
       </c>
       <c r="B575" s="12" t="s">
-        <v>1018</v>
+        <v>1289</v>
       </c>
       <c r="C575" s="12" t="s">
-        <v>1019</v>
+        <v>1290</v>
       </c>
       <c r="D575" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E575" s="12" t="s">
-        <v>4012</v>
+        <v>4011</v>
       </c>
       <c r="F575" s="12">
         <v>0</v>
@@ -27331,19 +27320,19 @@
     </row>
     <row r="576" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A576" s="12" t="s">
-        <v>248</v>
+        <v>545</v>
       </c>
       <c r="B576" s="12" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="C576" s="12" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="D576" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E576" s="12" t="s">
-        <v>4013</v>
+        <v>4012</v>
       </c>
       <c r="F576" s="12">
         <v>0</v>
@@ -27354,19 +27343,19 @@
     </row>
     <row r="577" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A577" s="12" t="s">
-        <v>168</v>
+        <v>248</v>
       </c>
       <c r="B577" s="12" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="C577" s="12" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="D577" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E577" s="12" t="s">
-        <v>4014</v>
+        <v>4013</v>
       </c>
       <c r="F577" s="12">
         <v>0</v>
@@ -27377,19 +27366,19 @@
     </row>
     <row r="578" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A578" s="12" t="s">
-        <v>243</v>
+        <v>168</v>
       </c>
       <c r="B578" s="12" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C578" s="12" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="D578" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E578" s="12" t="s">
-        <v>4015</v>
+        <v>4014</v>
       </c>
       <c r="F578" s="12">
         <v>0</v>
@@ -27400,19 +27389,19 @@
     </row>
     <row r="579" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A579" s="12" t="s">
-        <v>667</v>
+        <v>243</v>
       </c>
       <c r="B579" s="12" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="C579" s="12" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D579" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E579" s="12" t="s">
-        <v>4016</v>
+        <v>4015</v>
       </c>
       <c r="F579" s="12">
         <v>0</v>
@@ -27423,19 +27412,19 @@
     </row>
     <row r="580" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A580" s="12" t="s">
-        <v>691</v>
+        <v>667</v>
       </c>
       <c r="B580" s="12" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C580" s="12" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D580" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E580" s="12" t="s">
-        <v>4017</v>
+        <v>4016</v>
       </c>
       <c r="F580" s="12">
         <v>0</v>
@@ -27446,19 +27435,19 @@
     </row>
     <row r="581" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A581" s="12" t="s">
-        <v>650</v>
+        <v>691</v>
       </c>
       <c r="B581" s="12" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C581" s="12" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="D581" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E581" s="12" t="s">
-        <v>4018</v>
+        <v>4017</v>
       </c>
       <c r="F581" s="12">
         <v>0</v>
@@ -27469,19 +27458,19 @@
     </row>
     <row r="582" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A582" s="12" t="s">
-        <v>698</v>
+        <v>650</v>
       </c>
       <c r="B582" s="12" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C582" s="12" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D582" s="12" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E582" s="12" t="s">
-        <v>4019</v>
+        <v>4018</v>
       </c>
       <c r="F582" s="12">
         <v>0</v>
@@ -27492,19 +27481,19 @@
     </row>
     <row r="583" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A583" s="12" t="s">
-        <v>442</v>
+        <v>698</v>
       </c>
       <c r="B583" s="12" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C583" s="12" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="D583" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E583" s="12" t="s">
-        <v>4020</v>
+        <v>4019</v>
       </c>
       <c r="F583" s="12">
         <v>0</v>
@@ -27515,19 +27504,19 @@
     </row>
     <row r="584" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A584" s="12" t="s">
-        <v>209</v>
+        <v>442</v>
       </c>
       <c r="B584" s="12" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="C584" s="12" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="D584" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E584" s="12" t="s">
-        <v>4021</v>
+        <v>4020</v>
       </c>
       <c r="F584" s="12">
         <v>0</v>
@@ -27538,19 +27527,19 @@
     </row>
     <row r="585" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A585" s="12" t="s">
-        <v>662</v>
+        <v>209</v>
       </c>
       <c r="B585" s="12" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C585" s="12" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="D585" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E585" s="12" t="s">
-        <v>4022</v>
+        <v>4021</v>
       </c>
       <c r="F585" s="12">
         <v>0</v>
@@ -27561,19 +27550,19 @@
     </row>
     <row r="586" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A586" s="12" t="s">
-        <v>176</v>
+        <v>662</v>
       </c>
       <c r="B586" s="12" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="C586" s="12" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="D586" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E586" s="12" t="s">
-        <v>4023</v>
+        <v>4022</v>
       </c>
       <c r="F586" s="12">
         <v>0</v>
@@ -27584,19 +27573,19 @@
     </row>
     <row r="587" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A587" s="12" t="s">
-        <v>594</v>
+        <v>176</v>
       </c>
       <c r="B587" s="12" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="C587" s="12" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="D587" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E587" s="12" t="s">
-        <v>4024</v>
+        <v>4023</v>
       </c>
       <c r="F587" s="12">
         <v>0</v>
@@ -27607,19 +27596,19 @@
     </row>
     <row r="588" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A588" s="12" t="s">
-        <v>628</v>
+        <v>594</v>
       </c>
       <c r="B588" s="12" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C588" s="12" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="D588" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E588" s="12" t="s">
-        <v>4025</v>
+        <v>4024</v>
       </c>
       <c r="F588" s="12">
         <v>0</v>
@@ -27630,19 +27619,19 @@
     </row>
     <row r="589" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A589" s="12" t="s">
-        <v>443</v>
+        <v>628</v>
       </c>
       <c r="B589" s="12" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="C589" s="12" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D589" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E589" s="12" t="s">
-        <v>4026</v>
+        <v>4025</v>
       </c>
       <c r="F589" s="12">
         <v>0</v>
@@ -27653,19 +27642,19 @@
     </row>
     <row r="590" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A590" s="12" t="s">
-        <v>503</v>
+        <v>443</v>
       </c>
       <c r="B590" s="12" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="C590" s="12" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D590" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E590" s="12" t="s">
-        <v>4027</v>
+        <v>4026</v>
       </c>
       <c r="F590" s="12">
         <v>0</v>
@@ -27676,19 +27665,19 @@
     </row>
     <row r="591" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A591" s="12" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="B591" s="12" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="C591" s="12" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="D591" s="12" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E591" s="12" t="s">
-        <v>4028</v>
+        <v>4027</v>
       </c>
       <c r="F591" s="12">
         <v>0</v>
@@ -27699,19 +27688,19 @@
     </row>
     <row r="592" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A592" s="12" t="s">
-        <v>285</v>
+        <v>495</v>
       </c>
       <c r="B592" s="12" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C592" s="12" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="D592" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E592" s="12" t="s">
-        <v>4029</v>
+        <v>4028</v>
       </c>
       <c r="F592" s="12">
         <v>0</v>
@@ -27722,19 +27711,19 @@
     </row>
     <row r="593" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A593" s="12" t="s">
-        <v>128</v>
+        <v>285</v>
       </c>
       <c r="B593" s="12" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="C593" s="12" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="D593" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E593" s="12" t="s">
-        <v>4030</v>
+        <v>4029</v>
       </c>
       <c r="F593" s="12">
         <v>0</v>
@@ -27745,19 +27734,19 @@
     </row>
     <row r="594" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A594" s="12" t="s">
-        <v>657</v>
+        <v>128</v>
       </c>
       <c r="B594" s="12" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="C594" s="12" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="D594" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E594" s="12" t="s">
-        <v>4031</v>
+        <v>4030</v>
       </c>
       <c r="F594" s="12">
         <v>0</v>
@@ -27768,19 +27757,19 @@
     </row>
     <row r="595" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A595" s="12" t="s">
-        <v>144</v>
+        <v>657</v>
       </c>
       <c r="B595" s="12" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C595" s="12" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="D595" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E595" s="12" t="s">
-        <v>4032</v>
+        <v>4031</v>
       </c>
       <c r="F595" s="12">
         <v>0</v>
@@ -27791,19 +27780,19 @@
     </row>
     <row r="596" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A596" s="12" t="s">
-        <v>612</v>
+        <v>144</v>
       </c>
       <c r="B596" s="12" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C596" s="12" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="D596" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E596" s="12" t="s">
-        <v>4033</v>
+        <v>4032</v>
       </c>
       <c r="F596" s="12">
         <v>0</v>
@@ -27814,19 +27803,19 @@
     </row>
     <row r="597" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A597" s="12" t="s">
-        <v>203</v>
+        <v>612</v>
       </c>
       <c r="B597" s="12" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="C597" s="12" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="D597" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E597" s="12" t="s">
-        <v>4034</v>
+        <v>4033</v>
       </c>
       <c r="F597" s="12">
         <v>0</v>
@@ -27837,19 +27826,19 @@
     </row>
     <row r="598" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A598" s="12" t="s">
-        <v>624</v>
+        <v>203</v>
       </c>
       <c r="B598" s="12" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="C598" s="12" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="D598" s="12" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E598" s="12" t="s">
-        <v>4035</v>
+        <v>4034</v>
       </c>
       <c r="F598" s="12">
         <v>0</v>
@@ -27860,19 +27849,19 @@
     </row>
     <row r="599" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A599" s="12" t="s">
-        <v>163</v>
+        <v>624</v>
       </c>
       <c r="B599" s="12" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C599" s="12" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="D599" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E599" s="12" t="s">
-        <v>4036</v>
+        <v>4035</v>
       </c>
       <c r="F599" s="12">
         <v>0</v>
@@ -27883,19 +27872,19 @@
     </row>
     <row r="600" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A600" s="12" t="s">
-        <v>435</v>
+        <v>163</v>
       </c>
       <c r="B600" s="12" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="C600" s="12" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="D600" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E600" s="12" t="s">
-        <v>4037</v>
+        <v>4036</v>
       </c>
       <c r="F600" s="12">
         <v>0</v>
@@ -27906,19 +27895,19 @@
     </row>
     <row r="601" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A601" s="12" t="s">
-        <v>177</v>
+        <v>435</v>
       </c>
       <c r="B601" s="12" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="C601" s="12" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="D601" s="12" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E601" s="12" t="s">
-        <v>4038</v>
+        <v>4037</v>
       </c>
       <c r="F601" s="12">
         <v>0</v>
@@ -27929,19 +27918,19 @@
     </row>
     <row r="602" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A602" s="12" t="s">
-        <v>455</v>
+        <v>177</v>
       </c>
       <c r="B602" s="12" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="C602" s="12" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="D602" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E602" s="12" t="s">
-        <v>4039</v>
+        <v>4038</v>
       </c>
       <c r="F602" s="12">
         <v>0</v>
@@ -27952,19 +27941,19 @@
     </row>
     <row r="603" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A603" s="12" t="s">
-        <v>147</v>
+        <v>455</v>
       </c>
       <c r="B603" s="12" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="C603" s="12" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D603" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E603" s="12" t="s">
-        <v>4040</v>
+        <v>4039</v>
       </c>
       <c r="F603" s="12">
         <v>0</v>
@@ -27975,19 +27964,19 @@
     </row>
     <row r="604" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A604" s="12" t="s">
-        <v>627</v>
+        <v>147</v>
       </c>
       <c r="B604" s="12" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="C604" s="12" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D604" s="12" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E604" s="12" t="s">
-        <v>4041</v>
+        <v>4040</v>
       </c>
       <c r="F604" s="12">
         <v>0</v>
@@ -27998,62 +27987,62 @@
     </row>
     <row r="605" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A605" s="12" t="s">
-        <v>587</v>
+        <v>627</v>
       </c>
       <c r="B605" s="12" t="s">
-        <v>1078</v>
+        <v>1076</v>
+      </c>
+      <c r="C605" s="12" t="s">
+        <v>1077</v>
       </c>
       <c r="D605" s="12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E605" s="12" t="s">
-        <v>4042</v>
+        <v>4041</v>
       </c>
       <c r="F605" s="12">
         <v>0</v>
       </c>
       <c r="G605" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="606" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A606" s="12" t="s">
-        <v>164</v>
+        <v>587</v>
       </c>
       <c r="B606" s="12" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C606" s="12" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="D606" s="12" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E606" s="12" t="s">
-        <v>4043</v>
+        <v>4042</v>
       </c>
       <c r="F606" s="12">
         <v>0</v>
       </c>
       <c r="G606" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="607" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A607" s="12" t="s">
-        <v>255</v>
+        <v>164</v>
       </c>
       <c r="B607" s="12" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="C607" s="12" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="D607" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E607" s="12" t="s">
-        <v>4044</v>
+        <v>4043</v>
       </c>
       <c r="F607" s="12">
         <v>0</v>
@@ -28064,19 +28053,19 @@
     </row>
     <row r="608" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A608" s="12" t="s">
-        <v>392</v>
+        <v>255</v>
       </c>
       <c r="B608" s="12" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="C608" s="12" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D608" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E608" s="12" t="s">
-        <v>4045</v>
+        <v>4044</v>
       </c>
       <c r="F608" s="12">
         <v>0</v>
@@ -28087,19 +28076,19 @@
     </row>
     <row r="609" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A609" s="12" t="s">
-        <v>245</v>
+        <v>392</v>
       </c>
       <c r="B609" s="12" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="C609" s="12" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="D609" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E609" s="12" t="s">
-        <v>4046</v>
+        <v>4045</v>
       </c>
       <c r="F609" s="12">
         <v>0</v>
@@ -28110,19 +28099,19 @@
     </row>
     <row r="610" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A610" s="12" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B610" s="12" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="C610" s="12" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="D610" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E610" s="12" t="s">
-        <v>4047</v>
+        <v>4046</v>
       </c>
       <c r="F610" s="12">
         <v>0</v>
@@ -28133,19 +28122,19 @@
     </row>
     <row r="611" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A611" s="12" t="s">
-        <v>1291</v>
+        <v>220</v>
       </c>
       <c r="B611" s="12" t="s">
-        <v>1292</v>
+        <v>1087</v>
       </c>
       <c r="C611" s="12" t="s">
-        <v>1293</v>
+        <v>1088</v>
       </c>
       <c r="D611" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E611" s="12" t="s">
-        <v>4048</v>
+        <v>4047</v>
       </c>
       <c r="F611" s="12">
         <v>0</v>
@@ -28156,19 +28145,19 @@
     </row>
     <row r="612" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A612" s="12" t="s">
-        <v>190</v>
+        <v>1291</v>
       </c>
       <c r="B612" s="12" t="s">
-        <v>1089</v>
+        <v>1292</v>
       </c>
       <c r="C612" s="12" t="s">
-        <v>1090</v>
+        <v>1293</v>
       </c>
       <c r="D612" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E612" s="12" t="s">
-        <v>4049</v>
+        <v>4048</v>
       </c>
       <c r="F612" s="12">
         <v>0</v>
@@ -28179,16 +28168,19 @@
     </row>
     <row r="613" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A613" s="12" t="s">
-        <v>59</v>
+        <v>190</v>
       </c>
       <c r="B613" s="12" t="s">
-        <v>1091</v>
+        <v>1089</v>
+      </c>
+      <c r="C613" s="12" t="s">
+        <v>1090</v>
       </c>
       <c r="D613" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E613" s="12" t="s">
-        <v>4050</v>
+        <v>4049</v>
       </c>
       <c r="F613" s="12">
         <v>0</v>
@@ -28199,16 +28191,16 @@
     </row>
     <row r="614" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A614" s="12" t="s">
-        <v>193</v>
+        <v>59</v>
       </c>
       <c r="B614" s="12" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D614" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E614" s="12" t="s">
-        <v>4051</v>
+        <v>4050</v>
       </c>
       <c r="F614" s="12">
         <v>0</v>
@@ -28219,19 +28211,16 @@
     </row>
     <row r="615" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A615" s="12" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="B615" s="12" t="s">
-        <v>1093</v>
-      </c>
-      <c r="C615" s="12" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="D615" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E615" s="12" t="s">
-        <v>4052</v>
+        <v>4051</v>
       </c>
       <c r="F615" s="12">
         <v>0</v>
@@ -28242,19 +28231,19 @@
     </row>
     <row r="616" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A616" s="12" t="s">
-        <v>292</v>
+        <v>205</v>
       </c>
       <c r="B616" s="12" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C616" s="12" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="D616" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E616" s="12" t="s">
-        <v>4053</v>
+        <v>4052</v>
       </c>
       <c r="F616" s="12">
         <v>0</v>
@@ -28265,19 +28254,19 @@
     </row>
     <row r="617" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A617" s="12" t="s">
-        <v>557</v>
+        <v>292</v>
       </c>
       <c r="B617" s="12" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="C617" s="12" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="D617" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E617" s="12" t="s">
-        <v>4054</v>
+        <v>4053</v>
       </c>
       <c r="F617" s="12">
         <v>0</v>
@@ -28288,19 +28277,19 @@
     </row>
     <row r="618" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A618" s="12" t="s">
-        <v>318</v>
+        <v>557</v>
       </c>
       <c r="B618" s="12" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="C618" s="12" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="D618" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E618" s="12" t="s">
-        <v>4055</v>
+        <v>4054</v>
       </c>
       <c r="F618" s="12">
         <v>0</v>
@@ -28311,16 +28300,19 @@
     </row>
     <row r="619" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A619" s="12" t="s">
-        <v>201</v>
+        <v>318</v>
       </c>
       <c r="B619" s="12" t="s">
-        <v>1101</v>
+        <v>1099</v>
+      </c>
+      <c r="C619" s="12" t="s">
+        <v>1100</v>
       </c>
       <c r="D619" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E619" s="12" t="s">
-        <v>4056</v>
+        <v>4055</v>
       </c>
       <c r="F619" s="12">
         <v>0</v>
@@ -28331,19 +28323,16 @@
     </row>
     <row r="620" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A620" s="12" t="s">
-        <v>497</v>
+        <v>201</v>
       </c>
       <c r="B620" s="12" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C620" s="12" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="D620" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E620" s="12" t="s">
-        <v>4057</v>
+        <v>4056</v>
       </c>
       <c r="F620" s="12">
         <v>0</v>
@@ -28354,19 +28343,19 @@
     </row>
     <row r="621" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A621" s="12" t="s">
-        <v>559</v>
+        <v>497</v>
       </c>
       <c r="B621" s="12" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C621" s="12" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="D621" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E621" s="12" t="s">
-        <v>4058</v>
+        <v>4057</v>
       </c>
       <c r="F621" s="12">
         <v>0</v>
@@ -28377,19 +28366,19 @@
     </row>
     <row r="622" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A622" s="12" t="s">
-        <v>527</v>
+        <v>559</v>
       </c>
       <c r="B622" s="12" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C622" s="12" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="D622" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E622" s="12" t="s">
-        <v>4059</v>
+        <v>4058</v>
       </c>
       <c r="F622" s="12">
         <v>0</v>
@@ -28400,19 +28389,19 @@
     </row>
     <row r="623" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A623" s="12" t="s">
-        <v>293</v>
+        <v>527</v>
       </c>
       <c r="B623" s="12" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="C623" s="12" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="D623" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E623" s="12" t="s">
-        <v>4060</v>
+        <v>4059</v>
       </c>
       <c r="F623" s="12">
         <v>0</v>
@@ -28423,19 +28412,19 @@
     </row>
     <row r="624" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A624" s="12" t="s">
-        <v>447</v>
+        <v>293</v>
       </c>
       <c r="B624" s="12" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="C624" s="12" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="D624" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E624" s="12" t="s">
-        <v>4061</v>
+        <v>4060</v>
       </c>
       <c r="F624" s="12">
         <v>0</v>
@@ -28446,19 +28435,19 @@
     </row>
     <row r="625" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A625" s="12" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="B625" s="12" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C625" s="12" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="D625" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E625" s="12" t="s">
-        <v>4062</v>
+        <v>4061</v>
       </c>
       <c r="F625" s="12">
         <v>0</v>
@@ -28469,19 +28458,19 @@
     </row>
     <row r="626" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A626" s="12" t="s">
-        <v>333</v>
+        <v>460</v>
       </c>
       <c r="B626" s="12" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C626" s="12" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="D626" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E626" s="12" t="s">
-        <v>4063</v>
+        <v>4062</v>
       </c>
       <c r="F626" s="12">
         <v>0</v>
@@ -28492,19 +28481,19 @@
     </row>
     <row r="627" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A627" s="12" t="s">
-        <v>428</v>
+        <v>333</v>
       </c>
       <c r="B627" s="12" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C627" s="12" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="D627" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E627" s="12" t="s">
-        <v>4064</v>
+        <v>4063</v>
       </c>
       <c r="F627" s="12">
         <v>0</v>
@@ -28515,19 +28504,19 @@
     </row>
     <row r="628" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A628" s="12" t="s">
-        <v>537</v>
+        <v>428</v>
       </c>
       <c r="B628" s="12" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C628" s="12" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="D628" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E628" s="12" t="s">
-        <v>4065</v>
+        <v>4064</v>
       </c>
       <c r="F628" s="12">
         <v>0</v>
@@ -28538,19 +28527,19 @@
     </row>
     <row r="629" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A629" s="12" t="s">
-        <v>582</v>
+        <v>537</v>
       </c>
       <c r="B629" s="12" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="C629" s="12" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="D629" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E629" s="12" t="s">
-        <v>4066</v>
+        <v>4065</v>
       </c>
       <c r="F629" s="12">
         <v>0</v>
@@ -28561,19 +28550,19 @@
     </row>
     <row r="630" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A630" s="12" t="s">
-        <v>65</v>
+        <v>582</v>
       </c>
       <c r="B630" s="12" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="C630" s="12" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="D630" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E630" s="12" t="s">
-        <v>4067</v>
+        <v>4066</v>
       </c>
       <c r="F630" s="12">
         <v>0</v>
@@ -28584,19 +28573,19 @@
     </row>
     <row r="631" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A631" s="12" t="s">
-        <v>1294</v>
+        <v>65</v>
       </c>
       <c r="B631" s="12" t="s">
-        <v>1295</v>
+        <v>1122</v>
       </c>
       <c r="C631" s="12" t="s">
-        <v>1296</v>
+        <v>1123</v>
       </c>
       <c r="D631" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E631" s="12" t="s">
-        <v>4068</v>
+        <v>4067</v>
       </c>
       <c r="F631" s="12">
         <v>0</v>
@@ -28607,19 +28596,19 @@
     </row>
     <row r="632" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A632" s="12" t="s">
-        <v>1297</v>
+        <v>1294</v>
       </c>
       <c r="B632" s="12" t="s">
-        <v>1298</v>
+        <v>1295</v>
       </c>
       <c r="C632" s="12" t="s">
-        <v>1299</v>
+        <v>1296</v>
       </c>
       <c r="D632" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E632" s="12" t="s">
-        <v>4069</v>
+        <v>4068</v>
       </c>
       <c r="F632" s="12">
         <v>0</v>
@@ -28630,19 +28619,19 @@
     </row>
     <row r="633" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A633" s="12" t="s">
-        <v>99</v>
+        <v>1297</v>
       </c>
       <c r="B633" s="12" t="s">
-        <v>1124</v>
+        <v>1298</v>
       </c>
       <c r="C633" s="12" t="s">
-        <v>1125</v>
+        <v>1299</v>
       </c>
       <c r="D633" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E633" s="12" t="s">
-        <v>4070</v>
+        <v>4069</v>
       </c>
       <c r="F633" s="12">
         <v>0</v>
@@ -28653,19 +28642,19 @@
     </row>
     <row r="634" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A634" s="12" t="s">
-        <v>493</v>
+        <v>99</v>
       </c>
       <c r="B634" s="12" t="s">
-        <v>1300</v>
+        <v>1124</v>
       </c>
       <c r="C634" s="12" t="s">
-        <v>1301</v>
+        <v>1125</v>
       </c>
       <c r="D634" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E634" s="12" t="s">
-        <v>4071</v>
+        <v>4070</v>
       </c>
       <c r="F634" s="12">
         <v>0</v>
@@ -28676,19 +28665,19 @@
     </row>
     <row r="635" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A635" s="12" t="s">
-        <v>261</v>
+        <v>493</v>
       </c>
       <c r="B635" s="12" t="s">
-        <v>1126</v>
+        <v>1300</v>
       </c>
       <c r="C635" s="12" t="s">
-        <v>1127</v>
+        <v>1301</v>
       </c>
       <c r="D635" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E635" s="12" t="s">
-        <v>4072</v>
+        <v>4071</v>
       </c>
       <c r="F635" s="12">
         <v>0</v>
@@ -28699,19 +28688,19 @@
     </row>
     <row r="636" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A636" s="12" t="s">
-        <v>332</v>
+        <v>261</v>
       </c>
       <c r="B636" s="12" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="C636" s="12" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="D636" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E636" s="12" t="s">
-        <v>4073</v>
+        <v>4072</v>
       </c>
       <c r="F636" s="12">
         <v>0</v>
@@ -28722,62 +28711,62 @@
     </row>
     <row r="637" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A637" s="12" t="s">
-        <v>457</v>
+        <v>332</v>
       </c>
       <c r="B637" s="12" t="s">
-        <v>1130</v>
+        <v>1128</v>
+      </c>
+      <c r="C637" s="12" t="s">
+        <v>1129</v>
       </c>
       <c r="D637" s="12" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E637" s="12" t="s">
-        <v>4074</v>
+        <v>4073</v>
       </c>
       <c r="F637" s="12">
         <v>0</v>
       </c>
       <c r="G637" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="638" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A638" s="12" t="s">
-        <v>681</v>
+        <v>457</v>
       </c>
       <c r="B638" s="12" t="s">
-        <v>1131</v>
-      </c>
-      <c r="C638" s="12" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="D638" s="12" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E638" s="12" t="s">
-        <v>4075</v>
+        <v>4074</v>
       </c>
       <c r="F638" s="12">
         <v>0</v>
       </c>
       <c r="G638" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="639" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A639" s="12" t="s">
-        <v>4212</v>
+        <v>681</v>
       </c>
       <c r="B639" s="12" t="s">
-        <v>4168</v>
+        <v>1131</v>
       </c>
       <c r="C639" s="12" t="s">
-        <v>4169</v>
+        <v>1132</v>
       </c>
       <c r="D639" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E639" s="12" t="s">
-        <v>4193</v>
+        <v>4075</v>
       </c>
       <c r="F639" s="12">
         <v>0</v>
@@ -28788,19 +28777,19 @@
     </row>
     <row r="640" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A640" s="12" t="s">
-        <v>183</v>
+        <v>4212</v>
       </c>
       <c r="B640" s="12" t="s">
-        <v>1133</v>
+        <v>4168</v>
       </c>
       <c r="C640" s="12" t="s">
-        <v>1134</v>
+        <v>4169</v>
       </c>
       <c r="D640" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E640" s="12" t="s">
-        <v>4076</v>
+        <v>4193</v>
       </c>
       <c r="F640" s="12">
         <v>0</v>
@@ -28811,19 +28800,19 @@
     </row>
     <row r="641" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A641" s="12" t="s">
-        <v>446</v>
+        <v>183</v>
       </c>
       <c r="B641" s="12" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="C641" s="12" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="D641" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E641" s="12" t="s">
-        <v>4077</v>
+        <v>4076</v>
       </c>
       <c r="F641" s="12">
         <v>0</v>
@@ -28834,19 +28823,19 @@
     </row>
     <row r="642" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A642" s="12" t="s">
-        <v>697</v>
+        <v>446</v>
       </c>
       <c r="B642" s="12" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="C642" s="12" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="D642" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E642" s="12" t="s">
-        <v>4078</v>
+        <v>4077</v>
       </c>
       <c r="F642" s="12">
         <v>0</v>
@@ -28857,19 +28846,19 @@
     </row>
     <row r="643" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A643" s="12" t="s">
-        <v>685</v>
+        <v>697</v>
       </c>
       <c r="B643" s="12" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="C643" s="12" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="D643" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E643" s="12" t="s">
-        <v>4079</v>
+        <v>4078</v>
       </c>
       <c r="F643" s="12">
         <v>0</v>
@@ -28880,19 +28869,19 @@
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A644" s="12" t="s">
-        <v>673</v>
+        <v>685</v>
       </c>
       <c r="B644" s="12" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="C644" s="12" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="D644" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E644" s="12" t="s">
-        <v>4080</v>
+        <v>4079</v>
       </c>
       <c r="F644" s="12">
         <v>0</v>
@@ -28903,19 +28892,19 @@
     </row>
     <row r="645" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A645" s="12" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="B645" s="12" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="C645" s="12" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="D645" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E645" s="12" t="s">
-        <v>4081</v>
+        <v>4080</v>
       </c>
       <c r="F645" s="12">
         <v>0</v>
@@ -28926,19 +28915,19 @@
     </row>
     <row r="646" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A646" s="12" t="s">
-        <v>256</v>
+        <v>670</v>
       </c>
       <c r="B646" s="12" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="C646" s="12" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="D646" s="12" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E646" s="12" t="s">
-        <v>4082</v>
+        <v>4081</v>
       </c>
       <c r="F646" s="12">
         <v>0</v>
@@ -28949,19 +28938,19 @@
     </row>
     <row r="647" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A647" s="12" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B647" s="12" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="C647" s="12" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="D647" s="12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E647" s="12" t="s">
-        <v>4083</v>
+        <v>4082</v>
       </c>
       <c r="F647" s="12">
         <v>0</v>
@@ -28972,19 +28961,19 @@
     </row>
     <row r="648" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A648" s="12" t="s">
-        <v>575</v>
+        <v>267</v>
       </c>
       <c r="B648" s="12" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="C648" s="12" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="D648" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E648" s="12" t="s">
-        <v>4084</v>
+        <v>4083</v>
       </c>
       <c r="F648" s="12">
         <v>0</v>
@@ -28995,19 +28984,19 @@
     </row>
     <row r="649" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A649" s="12" t="s">
-        <v>538</v>
+        <v>575</v>
       </c>
       <c r="B649" s="12" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="C649" s="12" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="D649" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E649" s="12" t="s">
-        <v>4085</v>
+        <v>4084</v>
       </c>
       <c r="F649" s="12">
         <v>0</v>
@@ -29018,19 +29007,19 @@
     </row>
     <row r="650" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A650" s="12" t="s">
-        <v>370</v>
+        <v>538</v>
       </c>
       <c r="B650" s="12" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="C650" s="12" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="D650" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E650" s="12" t="s">
-        <v>4086</v>
+        <v>4085</v>
       </c>
       <c r="F650" s="12">
         <v>0</v>
@@ -29041,19 +29030,19 @@
     </row>
     <row r="651" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A651" s="12" t="s">
-        <v>334</v>
+        <v>370</v>
       </c>
       <c r="B651" s="12" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="C651" s="12" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="D651" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E651" s="12" t="s">
-        <v>4087</v>
+        <v>4086</v>
       </c>
       <c r="F651" s="12">
         <v>0</v>
@@ -29064,19 +29053,19 @@
     </row>
     <row r="652" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A652" s="12" t="s">
-        <v>613</v>
+        <v>334</v>
       </c>
       <c r="B652" s="12" t="s">
-        <v>1302</v>
+        <v>1155</v>
       </c>
       <c r="C652" s="12" t="s">
-        <v>1303</v>
+        <v>1156</v>
       </c>
       <c r="D652" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E652" s="12" t="s">
-        <v>4088</v>
+        <v>4087</v>
       </c>
       <c r="F652" s="12">
         <v>0</v>
@@ -29087,19 +29076,19 @@
     </row>
     <row r="653" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A653" s="12" t="s">
-        <v>102</v>
+        <v>613</v>
       </c>
       <c r="B653" s="12" t="s">
-        <v>1157</v>
+        <v>1302</v>
       </c>
       <c r="C653" s="12" t="s">
-        <v>1158</v>
+        <v>1303</v>
       </c>
       <c r="D653" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E653" s="12" t="s">
-        <v>4089</v>
+        <v>4088</v>
       </c>
       <c r="F653" s="12">
         <v>0</v>
@@ -29110,19 +29099,19 @@
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A654" s="12" t="s">
-        <v>466</v>
+        <v>102</v>
       </c>
       <c r="B654" s="12" t="s">
-        <v>1304</v>
+        <v>1157</v>
       </c>
       <c r="C654" s="12" t="s">
-        <v>1305</v>
+        <v>1158</v>
       </c>
       <c r="D654" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E654" s="12" t="s">
-        <v>4090</v>
+        <v>4089</v>
       </c>
       <c r="F654" s="12">
         <v>0</v>
@@ -29133,19 +29122,19 @@
     </row>
     <row r="655" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A655" s="12" t="s">
-        <v>109</v>
+        <v>466</v>
       </c>
       <c r="B655" s="12" t="s">
-        <v>1159</v>
+        <v>1304</v>
       </c>
       <c r="C655" s="12" t="s">
-        <v>1160</v>
+        <v>1305</v>
       </c>
       <c r="D655" s="12" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E655" s="12" t="s">
-        <v>4091</v>
+        <v>4090</v>
       </c>
       <c r="F655" s="12">
         <v>0</v>
@@ -29156,19 +29145,19 @@
     </row>
     <row r="656" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A656" s="12" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B656" s="12" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="C656" s="12" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="D656" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E656" s="12" t="s">
-        <v>4092</v>
+        <v>4091</v>
       </c>
       <c r="F656" s="12">
         <v>0</v>
@@ -29179,19 +29168,19 @@
     </row>
     <row r="657" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A657" s="12" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B657" s="12" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="C657" s="12" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="D657" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E657" s="12" t="s">
-        <v>4093</v>
+        <v>4092</v>
       </c>
       <c r="F657" s="12">
         <v>0</v>
@@ -29202,19 +29191,19 @@
     </row>
     <row r="658" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A658" s="12" t="s">
-        <v>477</v>
+        <v>110</v>
       </c>
       <c r="B658" s="12" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="C658" s="12" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="D658" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E658" s="12" t="s">
-        <v>4094</v>
+        <v>4093</v>
       </c>
       <c r="F658" s="12">
         <v>0</v>
@@ -29225,19 +29214,19 @@
     </row>
     <row r="659" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A659" s="12" t="s">
-        <v>216</v>
+        <v>477</v>
       </c>
       <c r="B659" s="12" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="C659" s="12" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="D659" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E659" s="12" t="s">
-        <v>4095</v>
+        <v>4094</v>
       </c>
       <c r="F659" s="12">
         <v>0</v>
@@ -29248,19 +29237,19 @@
     </row>
     <row r="660" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A660" s="12" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="B660" s="12" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="C660" s="12" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="D660" s="12" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E660" s="12" t="s">
-        <v>4096</v>
+        <v>4095</v>
       </c>
       <c r="F660" s="12">
         <v>0</v>
@@ -29271,19 +29260,19 @@
     </row>
     <row r="661" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A661" s="12" t="s">
-        <v>130</v>
+        <v>188</v>
       </c>
       <c r="B661" s="12" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="C661" s="12" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="D661" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E661" s="12" t="s">
-        <v>4097</v>
+        <v>4096</v>
       </c>
       <c r="F661" s="12">
         <v>0</v>
@@ -29294,19 +29283,19 @@
     </row>
     <row r="662" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A662" s="12" t="s">
-        <v>476</v>
+        <v>130</v>
       </c>
       <c r="B662" s="12" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="C662" s="12" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="D662" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E662" s="12" t="s">
-        <v>4098</v>
+        <v>4097</v>
       </c>
       <c r="F662" s="12">
         <v>0</v>
@@ -29317,19 +29306,19 @@
     </row>
     <row r="663" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A663" s="12" t="s">
-        <v>360</v>
+        <v>476</v>
       </c>
       <c r="B663" s="12" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="C663" s="12" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="D663" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E663" s="12" t="s">
-        <v>4099</v>
+        <v>4098</v>
       </c>
       <c r="F663" s="12">
         <v>0</v>
@@ -29340,19 +29329,19 @@
     </row>
     <row r="664" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A664" s="12" t="s">
-        <v>666</v>
+        <v>360</v>
       </c>
       <c r="B664" s="12" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="C664" s="12" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="D664" s="12" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E664" s="12" t="s">
-        <v>4100</v>
+        <v>4099</v>
       </c>
       <c r="F664" s="12">
         <v>0</v>
@@ -29363,19 +29352,19 @@
     </row>
     <row r="665" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A665" s="12" t="s">
-        <v>4213</v>
+        <v>666</v>
       </c>
       <c r="B665" s="12" t="s">
-        <v>4170</v>
+        <v>1177</v>
       </c>
       <c r="C665" s="12" t="s">
-        <v>4171</v>
+        <v>1178</v>
       </c>
       <c r="D665" s="12" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E665" s="12" t="s">
-        <v>4194</v>
+        <v>4100</v>
       </c>
       <c r="F665" s="12">
         <v>0</v>
@@ -29386,19 +29375,19 @@
     </row>
     <row r="666" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A666" s="12" t="s">
-        <v>1326</v>
+        <v>4213</v>
       </c>
       <c r="B666" s="12" t="s">
-        <v>1327</v>
+        <v>4170</v>
       </c>
       <c r="C666" s="12" t="s">
-        <v>1328</v>
+        <v>4171</v>
       </c>
       <c r="D666" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E666" s="12" t="s">
-        <v>4101</v>
+        <v>4194</v>
       </c>
       <c r="F666" s="12">
         <v>0</v>
@@ -29409,19 +29398,19 @@
     </row>
     <row r="667" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A667" s="12" t="s">
-        <v>4214</v>
+        <v>1326</v>
       </c>
       <c r="B667" s="12" t="s">
-        <v>4172</v>
+        <v>1327</v>
       </c>
       <c r="C667" s="12" t="s">
-        <v>4173</v>
+        <v>1328</v>
       </c>
       <c r="D667" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E667" s="12" t="s">
-        <v>4195</v>
+        <v>4101</v>
       </c>
       <c r="F667" s="12">
         <v>0</v>
@@ -29432,19 +29421,19 @@
     </row>
     <row r="668" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A668" s="12" t="s">
-        <v>4215</v>
+        <v>4214</v>
       </c>
       <c r="B668" s="12" t="s">
-        <v>4174</v>
+        <v>4172</v>
       </c>
       <c r="C668" s="12" t="s">
-        <v>4175</v>
+        <v>4173</v>
       </c>
       <c r="D668" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E668" s="12" t="s">
-        <v>4196</v>
+        <v>4195</v>
       </c>
       <c r="F668" s="12">
         <v>0</v>
@@ -29455,19 +29444,19 @@
     </row>
     <row r="669" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A669" s="12" t="s">
-        <v>273</v>
+        <v>4215</v>
       </c>
       <c r="B669" s="12" t="s">
-        <v>1179</v>
+        <v>4174</v>
       </c>
       <c r="C669" s="12" t="s">
-        <v>1180</v>
+        <v>4175</v>
       </c>
       <c r="D669" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E669" s="12" t="s">
-        <v>4102</v>
+        <v>4196</v>
       </c>
       <c r="F669" s="12">
         <v>0</v>
@@ -29478,19 +29467,19 @@
     </row>
     <row r="670" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A670" s="12" t="s">
-        <v>660</v>
+        <v>273</v>
       </c>
       <c r="B670" s="12" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C670" s="12" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="D670" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E670" s="12" t="s">
-        <v>4103</v>
+        <v>4102</v>
       </c>
       <c r="F670" s="12">
         <v>0</v>
@@ -29501,19 +29490,19 @@
     </row>
     <row r="671" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A671" s="12" t="s">
-        <v>95</v>
+        <v>660</v>
       </c>
       <c r="B671" s="12" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C671" s="12" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="D671" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E671" s="12" t="s">
-        <v>4104</v>
+        <v>4103</v>
       </c>
       <c r="F671" s="12">
         <v>0</v>
@@ -29524,19 +29513,19 @@
     </row>
     <row r="672" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A672" s="12" t="s">
-        <v>418</v>
+        <v>95</v>
       </c>
       <c r="B672" s="12" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C672" s="12" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="D672" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E672" s="12" t="s">
-        <v>4105</v>
+        <v>4104</v>
       </c>
       <c r="F672" s="12">
         <v>0</v>
@@ -29547,19 +29536,19 @@
     </row>
     <row r="673" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A673" s="12" t="s">
-        <v>380</v>
+        <v>418</v>
       </c>
       <c r="B673" s="12" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C673" s="12" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="D673" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E673" s="12" t="s">
-        <v>4106</v>
+        <v>4105</v>
       </c>
       <c r="F673" s="12">
         <v>0</v>
@@ -29570,19 +29559,19 @@
     </row>
     <row r="674" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A674" s="12" t="s">
-        <v>593</v>
+        <v>380</v>
       </c>
       <c r="B674" s="12" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="C674" s="12" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="D674" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E674" s="12" t="s">
-        <v>4107</v>
+        <v>4106</v>
       </c>
       <c r="F674" s="12">
         <v>0</v>
@@ -29593,16 +29582,19 @@
     </row>
     <row r="675" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A675" s="12" t="s">
-        <v>231</v>
+        <v>593</v>
       </c>
       <c r="B675" s="12" t="s">
-        <v>1191</v>
+        <v>1189</v>
+      </c>
+      <c r="C675" s="12" t="s">
+        <v>1190</v>
       </c>
       <c r="D675" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E675" s="12" t="s">
-        <v>4108</v>
+        <v>4107</v>
       </c>
       <c r="F675" s="12">
         <v>0</v>
@@ -29613,19 +29605,16 @@
     </row>
     <row r="676" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A676" s="12" t="s">
-        <v>606</v>
+        <v>231</v>
       </c>
       <c r="B676" s="12" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C676" s="12" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="D676" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E676" s="12" t="s">
-        <v>4109</v>
+        <v>4108</v>
       </c>
       <c r="F676" s="12">
         <v>0</v>
@@ -29636,19 +29625,19 @@
     </row>
     <row r="677" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A677" s="12" t="s">
-        <v>184</v>
+        <v>606</v>
       </c>
       <c r="B677" s="12" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="C677" s="12" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="D677" s="12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E677" s="12" t="s">
-        <v>4110</v>
+        <v>4109</v>
       </c>
       <c r="F677" s="12">
         <v>0</v>
@@ -29659,19 +29648,19 @@
     </row>
     <row r="678" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A678" s="12" t="s">
-        <v>329</v>
+        <v>184</v>
       </c>
       <c r="B678" s="12" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="C678" s="12" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="D678" s="12" t="s">
         <v>39</v>
       </c>
       <c r="E678" s="12" t="s">
-        <v>4111</v>
+        <v>4110</v>
       </c>
       <c r="F678" s="12">
         <v>0</v>
@@ -29682,19 +29671,19 @@
     </row>
     <row r="679" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A679" s="12" t="s">
-        <v>478</v>
+        <v>329</v>
       </c>
       <c r="B679" s="12" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="C679" s="12" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="D679" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E679" s="12" t="s">
-        <v>4112</v>
+        <v>4111</v>
       </c>
       <c r="F679" s="12">
         <v>0</v>
@@ -29705,19 +29694,19 @@
     </row>
     <row r="680" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A680" s="12" t="s">
-        <v>689</v>
+        <v>478</v>
       </c>
       <c r="B680" s="12" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="C680" s="12" t="s">
-        <v>1190</v>
+        <v>1199</v>
       </c>
       <c r="D680" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E680" s="12" t="s">
-        <v>4113</v>
+        <v>4112</v>
       </c>
       <c r="F680" s="12">
         <v>0</v>
@@ -29728,19 +29717,19 @@
     </row>
     <row r="681" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A681" s="12" t="s">
-        <v>104</v>
+        <v>689</v>
       </c>
       <c r="B681" s="12" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C681" s="12" t="s">
-        <v>1202</v>
+        <v>1190</v>
       </c>
       <c r="D681" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E681" s="12" t="s">
-        <v>4114</v>
+        <v>4113</v>
       </c>
       <c r="F681" s="12">
         <v>0</v>
@@ -29751,19 +29740,19 @@
     </row>
     <row r="682" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A682" s="12" t="s">
-        <v>636</v>
+        <v>104</v>
       </c>
       <c r="B682" s="12" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="C682" s="12" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="D682" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E682" s="12" t="s">
-        <v>4115</v>
+        <v>4114</v>
       </c>
       <c r="F682" s="12">
         <v>0</v>
@@ -29774,19 +29763,19 @@
     </row>
     <row r="683" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A683" s="12" t="s">
-        <v>621</v>
+        <v>636</v>
       </c>
       <c r="B683" s="12" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="C683" s="12" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="D683" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E683" s="12" t="s">
-        <v>4116</v>
+        <v>4115</v>
       </c>
       <c r="F683" s="12">
         <v>0</v>
@@ -29797,19 +29786,19 @@
     </row>
     <row r="684" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A684" s="12" t="s">
-        <v>120</v>
+        <v>621</v>
       </c>
       <c r="B684" s="12" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="C684" s="12" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="D684" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E684" s="12" t="s">
-        <v>4117</v>
+        <v>4116</v>
       </c>
       <c r="F684" s="12">
         <v>0</v>
@@ -29820,19 +29809,19 @@
     </row>
     <row r="685" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A685" s="12" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="B685" s="12" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="C685" s="12" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="D685" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E685" s="12" t="s">
-        <v>4118</v>
+        <v>4117</v>
       </c>
       <c r="F685" s="12">
         <v>0</v>
@@ -29843,16 +29832,19 @@
     </row>
     <row r="686" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A686" s="12" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="B686" s="12" t="s">
-        <v>1211</v>
+        <v>1209</v>
+      </c>
+      <c r="C686" s="12" t="s">
+        <v>1210</v>
       </c>
       <c r="D686" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E686" s="12" t="s">
-        <v>4119</v>
+        <v>4118</v>
       </c>
       <c r="F686" s="12">
         <v>0</v>
@@ -29863,19 +29855,16 @@
     </row>
     <row r="687" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A687" s="12" t="s">
-        <v>269</v>
+        <v>137</v>
       </c>
       <c r="B687" s="12" t="s">
-        <v>1212</v>
-      </c>
-      <c r="C687" s="12" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="D687" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E687" s="12" t="s">
-        <v>4120</v>
+        <v>4119</v>
       </c>
       <c r="F687" s="12">
         <v>0</v>
@@ -29886,19 +29875,19 @@
     </row>
     <row r="688" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A688" s="12" t="s">
-        <v>607</v>
+        <v>269</v>
       </c>
       <c r="B688" s="12" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="C688" s="12" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="D688" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E688" s="12" t="s">
-        <v>4121</v>
+        <v>4120</v>
       </c>
       <c r="F688" s="12">
         <v>0</v>
@@ -29909,19 +29898,19 @@
     </row>
     <row r="689" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A689" s="12" t="s">
-        <v>402</v>
+        <v>607</v>
       </c>
       <c r="B689" s="12" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="C689" s="12" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="D689" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E689" s="12" t="s">
-        <v>4122</v>
+        <v>4121</v>
       </c>
       <c r="F689" s="12">
         <v>0</v>
@@ -29932,19 +29921,19 @@
     </row>
     <row r="690" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A690" s="12" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B690" s="12" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="C690" s="12" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="D690" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E690" s="12" t="s">
-        <v>4123</v>
+        <v>4122</v>
       </c>
       <c r="F690" s="12">
         <v>0</v>
@@ -29955,19 +29944,19 @@
     </row>
     <row r="691" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A691" s="12" t="s">
-        <v>452</v>
+        <v>399</v>
       </c>
       <c r="B691" s="12" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="C691" s="12" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="D691" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E691" s="12" t="s">
-        <v>4124</v>
+        <v>4123</v>
       </c>
       <c r="F691" s="12">
         <v>0</v>
@@ -29978,19 +29967,19 @@
     </row>
     <row r="692" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A692" s="12" t="s">
-        <v>107</v>
+        <v>452</v>
       </c>
       <c r="B692" s="12" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="C692" s="12" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="D692" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E692" s="12" t="s">
-        <v>4125</v>
+        <v>4124</v>
       </c>
       <c r="F692" s="12">
         <v>0</v>
@@ -30001,16 +29990,19 @@
     </row>
     <row r="693" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A693" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B693" s="12" t="s">
-        <v>1224</v>
+        <v>1222</v>
+      </c>
+      <c r="C693" s="12" t="s">
+        <v>1223</v>
       </c>
       <c r="D693" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E693" s="12" t="s">
-        <v>4126</v>
+        <v>4125</v>
       </c>
       <c r="F693" s="12">
         <v>0</v>
@@ -30021,19 +30013,16 @@
     </row>
     <row r="694" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A694" s="12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B694" s="12" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C694" s="12" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="D694" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E694" s="12" t="s">
-        <v>4127</v>
+        <v>4126</v>
       </c>
       <c r="F694" s="12">
         <v>0</v>
@@ -30044,19 +30033,19 @@
     </row>
     <row r="695" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A695" s="12" t="s">
-        <v>554</v>
+        <v>118</v>
       </c>
       <c r="B695" s="12" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="C695" s="12" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="D695" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E695" s="12" t="s">
-        <v>4128</v>
+        <v>4127</v>
       </c>
       <c r="F695" s="12">
         <v>0</v>
@@ -30067,19 +30056,19 @@
     </row>
     <row r="696" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A696" s="12" t="s">
-        <v>192</v>
+        <v>554</v>
       </c>
       <c r="B696" s="12" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="C696" s="12" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="D696" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E696" s="12" t="s">
-        <v>4129</v>
+        <v>4128</v>
       </c>
       <c r="F696" s="12">
         <v>0</v>
@@ -30090,16 +30079,19 @@
     </row>
     <row r="697" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A697" s="12" t="s">
-        <v>278</v>
+        <v>192</v>
       </c>
       <c r="B697" s="12" t="s">
-        <v>1231</v>
+        <v>1229</v>
+      </c>
+      <c r="C697" s="12" t="s">
+        <v>1230</v>
       </c>
       <c r="D697" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E697" s="12" t="s">
-        <v>4130</v>
+        <v>4129</v>
       </c>
       <c r="F697" s="12">
         <v>0</v>
@@ -30110,19 +30102,16 @@
     </row>
     <row r="698" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A698" s="12" t="s">
-        <v>309</v>
+        <v>278</v>
       </c>
       <c r="B698" s="12" t="s">
-        <v>1232</v>
-      </c>
-      <c r="C698" s="12" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="D698" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E698" s="12" t="s">
-        <v>4131</v>
+        <v>4130</v>
       </c>
       <c r="F698" s="12">
         <v>0</v>
@@ -30133,19 +30122,19 @@
     </row>
     <row r="699" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A699" s="12" t="s">
-        <v>64</v>
+        <v>309</v>
       </c>
       <c r="B699" s="12" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="C699" s="12" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="D699" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E699" s="12" t="s">
-        <v>4132</v>
+        <v>4131</v>
       </c>
       <c r="F699" s="12">
         <v>0</v>
@@ -30156,19 +30145,19 @@
     </row>
     <row r="700" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A700" s="12" t="s">
-        <v>481</v>
+        <v>64</v>
       </c>
       <c r="B700" s="12" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="C700" s="12" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="D700" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E700" s="12" t="s">
-        <v>4133</v>
+        <v>4132</v>
       </c>
       <c r="F700" s="12">
         <v>0</v>
@@ -30179,62 +30168,62 @@
     </row>
     <row r="701" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A701" s="12" t="s">
-        <v>550</v>
+        <v>481</v>
       </c>
       <c r="B701" s="12" t="s">
-        <v>1238</v>
+        <v>1236</v>
+      </c>
+      <c r="C701" s="12" t="s">
+        <v>1237</v>
       </c>
       <c r="D701" s="12" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E701" s="12" t="s">
-        <v>4134</v>
+        <v>4133</v>
       </c>
       <c r="F701" s="12">
         <v>0</v>
       </c>
       <c r="G701" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="702" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A702" s="12" t="s">
-        <v>618</v>
+        <v>550</v>
       </c>
       <c r="B702" s="12" t="s">
-        <v>1239</v>
-      </c>
-      <c r="C702" s="12" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="D702" s="12" t="s">
         <v>35</v>
       </c>
       <c r="E702" s="12" t="s">
-        <v>4135</v>
+        <v>4134</v>
       </c>
       <c r="F702" s="12">
         <v>0</v>
       </c>
       <c r="G702" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="703" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A703" s="12" t="s">
-        <v>563</v>
+        <v>618</v>
       </c>
       <c r="B703" s="12" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="C703" s="12" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="D703" s="12" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E703" s="12" t="s">
-        <v>4136</v>
+        <v>4135</v>
       </c>
       <c r="F703" s="12">
         <v>0</v>
@@ -30245,29 +30234,56 @@
     </row>
     <row r="704" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A704" s="12" t="s">
-        <v>424</v>
+        <v>563</v>
       </c>
       <c r="B704" s="12" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="C704" s="12" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="D704" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E704" s="12" t="s">
+        <v>4136</v>
+      </c>
+      <c r="F704" s="12">
+        <v>0</v>
+      </c>
+      <c r="G704" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="705" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A705" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="B705" s="12" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C705" s="12" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D705" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E705" s="12" t="s">
         <v>4137</v>
       </c>
-      <c r="F704" s="12">
-        <v>0</v>
-      </c>
-      <c r="G704" s="12">
+      <c r="F705" s="12">
+        <v>0</v>
+      </c>
+      <c r="G705" s="12">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G704"/>
+  <autoFilter ref="A1:G705">
+    <sortState ref="A2:G706">
+      <sortCondition ref="A1:A706"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated dates of gazetteer data available. Added 2 more valid feature types to model
</commit_message>
<xml_diff>
--- a/GazetteerETL/Resources/UniversalGazetterModel.xlsx
+++ b/GazetteerETL/Resources/UniversalGazetterModel.xlsx
@@ -17,7 +17,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Country_Code!$A$1:$J$283</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Country_Code FIPS to ISO'!$A$1:$J$283</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FEATURE_CLASS!$A$1:$B$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FEATURE_CODE!$A$1:$G$705</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FEATURE_CODE!$A$1:$G$707</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PLACE_NAMES!$A$2:$D$21</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">Country_Code!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">'Country_Code FIPS to ISO'!$1:$1</definedName>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7621" uniqueCount="4297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7631" uniqueCount="4305">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -12918,6 +12918,30 @@
   </si>
   <si>
     <t>S-RSTNH</t>
+  </si>
+  <si>
+    <t>RRH</t>
+  </si>
+  <si>
+    <t>historical railroad</t>
+  </si>
+  <si>
+    <t>a former permanent twin steel-rail track on which freight and passenger cars move long distances</t>
+  </si>
+  <si>
+    <t>SYG</t>
+  </si>
+  <si>
+    <t>synagogue</t>
+  </si>
+  <si>
+    <t>a place for Jewish worship and religious instruction</t>
+  </si>
+  <si>
+    <t>S-SYG</t>
+  </si>
+  <si>
+    <t>R-RRH</t>
   </si>
 </sst>
 </file>
@@ -14231,17 +14255,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G705"/>
+  <dimension ref="A1:G707"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A708" sqref="A708"/>
+    <sheetView tabSelected="1" topLeftCell="A684" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" style="12" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.28515625" style="12" bestFit="1" customWidth="1"/>
@@ -26411,17 +26435,20 @@
       </c>
     </row>
     <row r="536" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A536" s="12" t="s">
-        <v>535</v>
-      </c>
-      <c r="B536" s="12" t="s">
-        <v>1688</v>
+      <c r="A536" s="10" t="s">
+        <v>4297</v>
+      </c>
+      <c r="B536" s="10" t="s">
+        <v>4298</v>
+      </c>
+      <c r="C536" s="10" t="s">
+        <v>4299</v>
       </c>
       <c r="D536" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E536" s="12" t="s">
-        <v>3975</v>
+        <v>4304</v>
       </c>
       <c r="F536" s="12">
         <v>0</v>
@@ -26432,19 +26459,16 @@
     </row>
     <row r="537" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A537" s="12" t="s">
-        <v>317</v>
+        <v>535</v>
       </c>
       <c r="B537" s="12" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C537" s="12" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="D537" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E537" s="12" t="s">
-        <v>3976</v>
+        <v>3975</v>
       </c>
       <c r="F537" s="12">
         <v>0</v>
@@ -26455,19 +26479,19 @@
     </row>
     <row r="538" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A538" s="12" t="s">
-        <v>472</v>
+        <v>317</v>
       </c>
       <c r="B538" s="12" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="C538" s="12" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="D538" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E538" s="12" t="s">
-        <v>3977</v>
+        <v>3976</v>
       </c>
       <c r="F538" s="12">
         <v>0</v>
@@ -26478,19 +26502,19 @@
     </row>
     <row r="539" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A539" s="12" t="s">
-        <v>121</v>
+        <v>472</v>
       </c>
       <c r="B539" s="12" t="s">
-        <v>718</v>
+        <v>1691</v>
       </c>
       <c r="C539" s="12" t="s">
-        <v>719</v>
+        <v>1692</v>
       </c>
       <c r="D539" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E539" s="12" t="s">
-        <v>3978</v>
+        <v>3977</v>
       </c>
       <c r="F539" s="12">
         <v>0</v>
@@ -26501,19 +26525,19 @@
     </row>
     <row r="540" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A540" s="12" t="s">
-        <v>276</v>
+        <v>121</v>
       </c>
       <c r="B540" s="12" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="C540" s="12" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="D540" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E540" s="12" t="s">
-        <v>3979</v>
+        <v>3978</v>
       </c>
       <c r="F540" s="12">
         <v>0</v>
@@ -26524,19 +26548,19 @@
     </row>
     <row r="541" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A541" s="12" t="s">
-        <v>4293</v>
+        <v>276</v>
       </c>
       <c r="B541" s="12" t="s">
-        <v>4294</v>
+        <v>720</v>
       </c>
       <c r="C541" s="12" t="s">
-        <v>4295</v>
+        <v>721</v>
       </c>
       <c r="D541" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E541" s="12" t="s">
-        <v>4296</v>
+        <v>3979</v>
       </c>
       <c r="F541" s="12">
         <v>0</v>
@@ -26547,16 +26571,19 @@
     </row>
     <row r="542" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A542" s="12" t="s">
-        <v>295</v>
+        <v>4293</v>
       </c>
       <c r="B542" s="12" t="s">
-        <v>722</v>
+        <v>4294</v>
+      </c>
+      <c r="C542" s="12" t="s">
+        <v>4295</v>
       </c>
       <c r="D542" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E542" s="12" t="s">
-        <v>3980</v>
+        <v>4296</v>
       </c>
       <c r="F542" s="12">
         <v>0</v>
@@ -26567,19 +26594,16 @@
     </row>
     <row r="543" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A543" s="12" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="B543" s="12" t="s">
-        <v>723</v>
-      </c>
-      <c r="C543" s="12" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D543" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E543" s="12" t="s">
-        <v>3981</v>
+        <v>3980</v>
       </c>
       <c r="F543" s="12">
         <v>0</v>
@@ -26590,16 +26614,19 @@
     </row>
     <row r="544" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A544" s="12" t="s">
-        <v>584</v>
+        <v>284</v>
       </c>
       <c r="B544" s="12" t="s">
-        <v>725</v>
+        <v>723</v>
+      </c>
+      <c r="C544" s="12" t="s">
+        <v>724</v>
       </c>
       <c r="D544" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E544" s="12" t="s">
-        <v>3982</v>
+        <v>3981</v>
       </c>
       <c r="F544" s="12">
         <v>0</v>
@@ -26610,19 +26637,16 @@
     </row>
     <row r="545" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A545" s="12" t="s">
-        <v>101</v>
+        <v>584</v>
       </c>
       <c r="B545" s="12" t="s">
-        <v>726</v>
-      </c>
-      <c r="C545" s="12" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D545" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E545" s="12" t="s">
-        <v>3983</v>
+        <v>3982</v>
       </c>
       <c r="F545" s="12">
         <v>0</v>
@@ -26633,16 +26657,19 @@
     </row>
     <row r="546" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A546" s="12" t="s">
-        <v>514</v>
+        <v>101</v>
       </c>
       <c r="B546" s="12" t="s">
-        <v>728</v>
+        <v>726</v>
+      </c>
+      <c r="C546" s="12" t="s">
+        <v>727</v>
       </c>
       <c r="D546" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E546" s="12" t="s">
-        <v>3984</v>
+        <v>3983</v>
       </c>
       <c r="F546" s="12">
         <v>0</v>
@@ -26653,19 +26680,16 @@
     </row>
     <row r="547" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A547" s="12" t="s">
-        <v>199</v>
+        <v>514</v>
       </c>
       <c r="B547" s="12" t="s">
-        <v>729</v>
-      </c>
-      <c r="C547" s="12" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D547" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E547" s="12" t="s">
-        <v>3985</v>
+        <v>3984</v>
       </c>
       <c r="F547" s="12">
         <v>0</v>
@@ -26676,19 +26700,19 @@
     </row>
     <row r="548" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A548" s="12" t="s">
-        <v>252</v>
+        <v>199</v>
       </c>
       <c r="B548" s="12" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="C548" s="12" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D548" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E548" s="12" t="s">
-        <v>3986</v>
+        <v>3985</v>
       </c>
       <c r="F548" s="12">
         <v>0</v>
@@ -26699,19 +26723,19 @@
     </row>
     <row r="549" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A549" s="12" t="s">
-        <v>115</v>
+        <v>252</v>
       </c>
       <c r="B549" s="12" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="C549" s="12" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D549" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E549" s="12" t="s">
-        <v>3987</v>
+        <v>3986</v>
       </c>
       <c r="F549" s="12">
         <v>0</v>
@@ -26722,19 +26746,19 @@
     </row>
     <row r="550" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A550" s="12" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B550" s="12" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="C550" s="12" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D550" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E550" s="12" t="s">
-        <v>3988</v>
+        <v>3987</v>
       </c>
       <c r="F550" s="12">
         <v>0</v>
@@ -26745,19 +26769,19 @@
     </row>
     <row r="551" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A551" s="12" t="s">
-        <v>417</v>
+        <v>165</v>
       </c>
       <c r="B551" s="12" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="C551" s="12" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D551" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E551" s="12" t="s">
-        <v>3989</v>
+        <v>3988</v>
       </c>
       <c r="F551" s="12">
         <v>0</v>
@@ -26768,19 +26792,19 @@
     </row>
     <row r="552" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A552" s="12" t="s">
-        <v>132</v>
+        <v>417</v>
       </c>
       <c r="B552" s="12" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C552" s="12" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D552" s="12" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E552" s="12" t="s">
-        <v>3990</v>
+        <v>3989</v>
       </c>
       <c r="F552" s="12">
         <v>0</v>
@@ -26791,19 +26815,19 @@
     </row>
     <row r="553" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A553" s="12" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
       <c r="B553" s="12" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="C553" s="12" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="D553" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E553" s="12" t="s">
-        <v>3991</v>
+        <v>3990</v>
       </c>
       <c r="F553" s="12">
         <v>0</v>
@@ -26814,19 +26838,19 @@
     </row>
     <row r="554" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A554" s="12" t="s">
-        <v>211</v>
+        <v>108</v>
       </c>
       <c r="B554" s="12" t="s">
-        <v>983</v>
+        <v>741</v>
       </c>
       <c r="C554" s="12" t="s">
-        <v>984</v>
+        <v>742</v>
       </c>
       <c r="D554" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E554" s="12" t="s">
-        <v>3992</v>
+        <v>3991</v>
       </c>
       <c r="F554" s="12">
         <v>0</v>
@@ -26837,19 +26861,19 @@
     </row>
     <row r="555" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A555" s="12" t="s">
-        <v>122</v>
+        <v>211</v>
       </c>
       <c r="B555" s="12" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="C555" s="12" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="D555" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E555" s="12" t="s">
-        <v>3993</v>
+        <v>3992</v>
       </c>
       <c r="F555" s="12">
         <v>0</v>
@@ -26860,19 +26884,19 @@
     </row>
     <row r="556" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A556" s="12" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="B556" s="12" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="C556" s="12" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D556" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E556" s="12" t="s">
-        <v>3994</v>
+        <v>3993</v>
       </c>
       <c r="F556" s="12">
         <v>0</v>
@@ -26883,19 +26907,19 @@
     </row>
     <row r="557" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A557" s="12" t="s">
-        <v>384</v>
+        <v>170</v>
       </c>
       <c r="B557" s="12" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="C557" s="12" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="D557" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E557" s="12" t="s">
-        <v>3995</v>
+        <v>3994</v>
       </c>
       <c r="F557" s="12">
         <v>0</v>
@@ -26906,19 +26930,19 @@
     </row>
     <row r="558" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A558" s="12" t="s">
-        <v>429</v>
+        <v>384</v>
       </c>
       <c r="B558" s="12" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C558" s="12" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="D558" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E558" s="12" t="s">
-        <v>3996</v>
+        <v>3995</v>
       </c>
       <c r="F558" s="12">
         <v>0</v>
@@ -26929,19 +26953,19 @@
     </row>
     <row r="559" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A559" s="12" t="s">
-        <v>4210</v>
+        <v>429</v>
       </c>
       <c r="B559" s="12" t="s">
-        <v>4164</v>
+        <v>991</v>
       </c>
       <c r="C559" s="12" t="s">
-        <v>4165</v>
+        <v>992</v>
       </c>
       <c r="D559" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E559" s="12" t="s">
-        <v>4191</v>
+        <v>3996</v>
       </c>
       <c r="F559" s="12">
         <v>0</v>
@@ -26952,19 +26976,19 @@
     </row>
     <row r="560" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A560" s="12" t="s">
-        <v>487</v>
+        <v>4210</v>
       </c>
       <c r="B560" s="12" t="s">
-        <v>993</v>
+        <v>4164</v>
       </c>
       <c r="C560" s="12" t="s">
-        <v>994</v>
+        <v>4165</v>
       </c>
       <c r="D560" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E560" s="12" t="s">
-        <v>3997</v>
+        <v>4191</v>
       </c>
       <c r="F560" s="12">
         <v>0</v>
@@ -26975,19 +26999,19 @@
     </row>
     <row r="561" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A561" s="12" t="s">
-        <v>601</v>
+        <v>487</v>
       </c>
       <c r="B561" s="12" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C561" s="12" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="D561" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E561" s="12" t="s">
-        <v>3998</v>
+        <v>3997</v>
       </c>
       <c r="F561" s="12">
         <v>0</v>
@@ -26998,19 +27022,19 @@
     </row>
     <row r="562" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A562" s="12" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="B562" s="12" t="s">
-        <v>1286</v>
+        <v>995</v>
       </c>
       <c r="C562" s="12" t="s">
-        <v>1287</v>
+        <v>996</v>
       </c>
       <c r="D562" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E562" s="12" t="s">
-        <v>3999</v>
+        <v>3998</v>
       </c>
       <c r="F562" s="12">
         <v>0</v>
@@ -27021,19 +27045,19 @@
     </row>
     <row r="563" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A563" s="12" t="s">
-        <v>688</v>
+        <v>609</v>
       </c>
       <c r="B563" s="12" t="s">
-        <v>997</v>
+        <v>1286</v>
       </c>
       <c r="C563" s="12" t="s">
-        <v>998</v>
+        <v>1287</v>
       </c>
       <c r="D563" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E563" s="12" t="s">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="F563" s="12">
         <v>0</v>
@@ -27044,19 +27068,19 @@
     </row>
     <row r="564" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A564" s="12" t="s">
-        <v>160</v>
+        <v>688</v>
       </c>
       <c r="B564" s="12" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="C564" s="12" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D564" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E564" s="12" t="s">
-        <v>4001</v>
+        <v>4000</v>
       </c>
       <c r="F564" s="12">
         <v>0</v>
@@ -27067,19 +27091,19 @@
     </row>
     <row r="565" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A565" s="12" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B565" s="12" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="C565" s="12" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D565" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E565" s="12" t="s">
-        <v>4002</v>
+        <v>4001</v>
       </c>
       <c r="F565" s="12">
         <v>0</v>
@@ -27090,19 +27114,19 @@
     </row>
     <row r="566" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A566" s="12" t="s">
-        <v>699</v>
+        <v>155</v>
       </c>
       <c r="B566" s="12" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="C566" s="12" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D566" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E566" s="12" t="s">
-        <v>4003</v>
+        <v>4002</v>
       </c>
       <c r="F566" s="12">
         <v>0</v>
@@ -27113,19 +27137,19 @@
     </row>
     <row r="567" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A567" s="12" t="s">
-        <v>389</v>
+        <v>699</v>
       </c>
       <c r="B567" s="12" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="C567" s="12" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D567" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E567" s="12" t="s">
-        <v>4004</v>
+        <v>4003</v>
       </c>
       <c r="F567" s="12">
         <v>0</v>
@@ -27136,19 +27160,19 @@
     </row>
     <row r="568" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A568" s="12" t="s">
-        <v>249</v>
+        <v>389</v>
       </c>
       <c r="B568" s="12" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="C568" s="12" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D568" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E568" s="12" t="s">
-        <v>4005</v>
+        <v>4004</v>
       </c>
       <c r="F568" s="12">
         <v>0</v>
@@ -27159,19 +27183,19 @@
     </row>
     <row r="569" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A569" s="12" t="s">
-        <v>679</v>
+        <v>249</v>
       </c>
       <c r="B569" s="12" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="C569" s="12" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D569" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E569" s="12" t="s">
-        <v>4006</v>
+        <v>4005</v>
       </c>
       <c r="F569" s="12">
         <v>0</v>
@@ -27182,65 +27206,65 @@
     </row>
     <row r="570" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A570" s="12" t="s">
-        <v>396</v>
+        <v>679</v>
       </c>
       <c r="B570" s="12" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="C570" s="12" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D570" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E570" s="12" t="s">
-        <v>4007</v>
+        <v>4006</v>
       </c>
       <c r="F570" s="12">
         <v>0</v>
       </c>
       <c r="G570" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="571" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A571" s="12" t="s">
-        <v>4211</v>
+        <v>396</v>
       </c>
       <c r="B571" s="12" t="s">
-        <v>4166</v>
+        <v>1011</v>
       </c>
       <c r="C571" s="12" t="s">
-        <v>4167</v>
+        <v>1012</v>
       </c>
       <c r="D571" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E571" s="12" t="s">
-        <v>4192</v>
+        <v>4007</v>
       </c>
       <c r="F571" s="12">
         <v>0</v>
       </c>
       <c r="G571" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="572" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A572" s="12" t="s">
-        <v>687</v>
+        <v>4211</v>
       </c>
       <c r="B572" s="12" t="s">
-        <v>1013</v>
+        <v>4166</v>
       </c>
       <c r="C572" s="12" t="s">
-        <v>1014</v>
+        <v>4167</v>
       </c>
       <c r="D572" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E572" s="12" t="s">
-        <v>4008</v>
+        <v>4192</v>
       </c>
       <c r="F572" s="12">
         <v>0</v>
@@ -27251,19 +27275,19 @@
     </row>
     <row r="573" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A573" s="12" t="s">
-        <v>603</v>
+        <v>687</v>
       </c>
       <c r="B573" s="12" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="C573" s="12" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="D573" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E573" s="12" t="s">
-        <v>4009</v>
+        <v>4008</v>
       </c>
       <c r="F573" s="12">
         <v>0</v>
@@ -27274,19 +27298,19 @@
     </row>
     <row r="574" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A574" s="12" t="s">
-        <v>82</v>
+        <v>603</v>
       </c>
       <c r="B574" s="12" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="C574" s="12" t="s">
         <v>1016</v>
       </c>
       <c r="D574" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E574" s="12" t="s">
-        <v>4010</v>
+        <v>4009</v>
       </c>
       <c r="F574" s="12">
         <v>0</v>
@@ -27297,19 +27321,19 @@
     </row>
     <row r="575" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A575" s="12" t="s">
-        <v>1288</v>
+        <v>82</v>
       </c>
       <c r="B575" s="12" t="s">
-        <v>1289</v>
+        <v>1017</v>
       </c>
       <c r="C575" s="12" t="s">
-        <v>1290</v>
+        <v>1016</v>
       </c>
       <c r="D575" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E575" s="12" t="s">
-        <v>4011</v>
+        <v>4010</v>
       </c>
       <c r="F575" s="12">
         <v>0</v>
@@ -27320,19 +27344,19 @@
     </row>
     <row r="576" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A576" s="12" t="s">
-        <v>545</v>
+        <v>1288</v>
       </c>
       <c r="B576" s="12" t="s">
-        <v>1018</v>
+        <v>1289</v>
       </c>
       <c r="C576" s="12" t="s">
-        <v>1019</v>
+        <v>1290</v>
       </c>
       <c r="D576" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E576" s="12" t="s">
-        <v>4012</v>
+        <v>4011</v>
       </c>
       <c r="F576" s="12">
         <v>0</v>
@@ -27343,19 +27367,19 @@
     </row>
     <row r="577" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A577" s="12" t="s">
-        <v>248</v>
+        <v>545</v>
       </c>
       <c r="B577" s="12" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="C577" s="12" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="D577" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E577" s="12" t="s">
-        <v>4013</v>
+        <v>4012</v>
       </c>
       <c r="F577" s="12">
         <v>0</v>
@@ -27366,19 +27390,19 @@
     </row>
     <row r="578" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A578" s="12" t="s">
-        <v>168</v>
+        <v>248</v>
       </c>
       <c r="B578" s="12" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="C578" s="12" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="D578" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E578" s="12" t="s">
-        <v>4014</v>
+        <v>4013</v>
       </c>
       <c r="F578" s="12">
         <v>0</v>
@@ -27389,19 +27413,19 @@
     </row>
     <row r="579" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A579" s="12" t="s">
-        <v>243</v>
+        <v>168</v>
       </c>
       <c r="B579" s="12" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="C579" s="12" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="D579" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E579" s="12" t="s">
-        <v>4015</v>
+        <v>4014</v>
       </c>
       <c r="F579" s="12">
         <v>0</v>
@@ -27412,19 +27436,19 @@
     </row>
     <row r="580" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A580" s="12" t="s">
-        <v>667</v>
+        <v>243</v>
       </c>
       <c r="B580" s="12" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="C580" s="12" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D580" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E580" s="12" t="s">
-        <v>4016</v>
+        <v>4015</v>
       </c>
       <c r="F580" s="12">
         <v>0</v>
@@ -27435,19 +27459,19 @@
     </row>
     <row r="581" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A581" s="12" t="s">
-        <v>691</v>
+        <v>667</v>
       </c>
       <c r="B581" s="12" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C581" s="12" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D581" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E581" s="12" t="s">
-        <v>4017</v>
+        <v>4016</v>
       </c>
       <c r="F581" s="12">
         <v>0</v>
@@ -27458,19 +27482,19 @@
     </row>
     <row r="582" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A582" s="12" t="s">
-        <v>650</v>
+        <v>691</v>
       </c>
       <c r="B582" s="12" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C582" s="12" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="D582" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E582" s="12" t="s">
-        <v>4018</v>
+        <v>4017</v>
       </c>
       <c r="F582" s="12">
         <v>0</v>
@@ -27481,19 +27505,19 @@
     </row>
     <row r="583" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A583" s="12" t="s">
-        <v>698</v>
+        <v>650</v>
       </c>
       <c r="B583" s="12" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C583" s="12" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D583" s="12" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E583" s="12" t="s">
-        <v>4019</v>
+        <v>4018</v>
       </c>
       <c r="F583" s="12">
         <v>0</v>
@@ -27504,19 +27528,19 @@
     </row>
     <row r="584" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A584" s="12" t="s">
-        <v>442</v>
+        <v>698</v>
       </c>
       <c r="B584" s="12" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="C584" s="12" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="D584" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E584" s="12" t="s">
-        <v>4020</v>
+        <v>4019</v>
       </c>
       <c r="F584" s="12">
         <v>0</v>
@@ -27527,19 +27551,19 @@
     </row>
     <row r="585" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A585" s="12" t="s">
-        <v>209</v>
+        <v>442</v>
       </c>
       <c r="B585" s="12" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="C585" s="12" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="D585" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E585" s="12" t="s">
-        <v>4021</v>
+        <v>4020</v>
       </c>
       <c r="F585" s="12">
         <v>0</v>
@@ -27550,19 +27574,19 @@
     </row>
     <row r="586" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A586" s="12" t="s">
-        <v>662</v>
+        <v>209</v>
       </c>
       <c r="B586" s="12" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C586" s="12" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="D586" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E586" s="12" t="s">
-        <v>4022</v>
+        <v>4021</v>
       </c>
       <c r="F586" s="12">
         <v>0</v>
@@ -27573,19 +27597,19 @@
     </row>
     <row r="587" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A587" s="12" t="s">
-        <v>176</v>
+        <v>662</v>
       </c>
       <c r="B587" s="12" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="C587" s="12" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="D587" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E587" s="12" t="s">
-        <v>4023</v>
+        <v>4022</v>
       </c>
       <c r="F587" s="12">
         <v>0</v>
@@ -27596,19 +27620,19 @@
     </row>
     <row r="588" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A588" s="12" t="s">
-        <v>594</v>
+        <v>176</v>
       </c>
       <c r="B588" s="12" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="C588" s="12" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="D588" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E588" s="12" t="s">
-        <v>4024</v>
+        <v>4023</v>
       </c>
       <c r="F588" s="12">
         <v>0</v>
@@ -27619,19 +27643,19 @@
     </row>
     <row r="589" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A589" s="12" t="s">
-        <v>628</v>
+        <v>594</v>
       </c>
       <c r="B589" s="12" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C589" s="12" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="D589" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E589" s="12" t="s">
-        <v>4025</v>
+        <v>4024</v>
       </c>
       <c r="F589" s="12">
         <v>0</v>
@@ -27642,19 +27666,19 @@
     </row>
     <row r="590" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A590" s="12" t="s">
-        <v>443</v>
+        <v>628</v>
       </c>
       <c r="B590" s="12" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="C590" s="12" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D590" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E590" s="12" t="s">
-        <v>4026</v>
+        <v>4025</v>
       </c>
       <c r="F590" s="12">
         <v>0</v>
@@ -27665,19 +27689,19 @@
     </row>
     <row r="591" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A591" s="12" t="s">
-        <v>503</v>
+        <v>443</v>
       </c>
       <c r="B591" s="12" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="C591" s="12" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D591" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E591" s="12" t="s">
-        <v>4027</v>
+        <v>4026</v>
       </c>
       <c r="F591" s="12">
         <v>0</v>
@@ -27688,19 +27712,19 @@
     </row>
     <row r="592" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A592" s="12" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="B592" s="12" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="C592" s="12" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="D592" s="12" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E592" s="12" t="s">
-        <v>4028</v>
+        <v>4027</v>
       </c>
       <c r="F592" s="12">
         <v>0</v>
@@ -27711,19 +27735,19 @@
     </row>
     <row r="593" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A593" s="12" t="s">
-        <v>285</v>
+        <v>495</v>
       </c>
       <c r="B593" s="12" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="C593" s="12" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="D593" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E593" s="12" t="s">
-        <v>4029</v>
+        <v>4028</v>
       </c>
       <c r="F593" s="12">
         <v>0</v>
@@ -27734,19 +27758,19 @@
     </row>
     <row r="594" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A594" s="12" t="s">
-        <v>128</v>
+        <v>285</v>
       </c>
       <c r="B594" s="12" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="C594" s="12" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="D594" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E594" s="12" t="s">
-        <v>4030</v>
+        <v>4029</v>
       </c>
       <c r="F594" s="12">
         <v>0</v>
@@ -27757,19 +27781,19 @@
     </row>
     <row r="595" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A595" s="12" t="s">
-        <v>657</v>
+        <v>128</v>
       </c>
       <c r="B595" s="12" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="C595" s="12" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="D595" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E595" s="12" t="s">
-        <v>4031</v>
+        <v>4030</v>
       </c>
       <c r="F595" s="12">
         <v>0</v>
@@ -27780,19 +27804,19 @@
     </row>
     <row r="596" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A596" s="12" t="s">
-        <v>144</v>
+        <v>657</v>
       </c>
       <c r="B596" s="12" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="C596" s="12" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="D596" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E596" s="12" t="s">
-        <v>4032</v>
+        <v>4031</v>
       </c>
       <c r="F596" s="12">
         <v>0</v>
@@ -27803,19 +27827,19 @@
     </row>
     <row r="597" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A597" s="12" t="s">
-        <v>612</v>
+        <v>144</v>
       </c>
       <c r="B597" s="12" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="C597" s="12" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="D597" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E597" s="12" t="s">
-        <v>4033</v>
+        <v>4032</v>
       </c>
       <c r="F597" s="12">
         <v>0</v>
@@ -27826,19 +27850,19 @@
     </row>
     <row r="598" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A598" s="12" t="s">
-        <v>203</v>
+        <v>612</v>
       </c>
       <c r="B598" s="12" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="C598" s="12" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="D598" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E598" s="12" t="s">
-        <v>4034</v>
+        <v>4033</v>
       </c>
       <c r="F598" s="12">
         <v>0</v>
@@ -27849,19 +27873,19 @@
     </row>
     <row r="599" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A599" s="12" t="s">
-        <v>624</v>
+        <v>203</v>
       </c>
       <c r="B599" s="12" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="C599" s="12" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="D599" s="12" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E599" s="12" t="s">
-        <v>4035</v>
+        <v>4034</v>
       </c>
       <c r="F599" s="12">
         <v>0</v>
@@ -27872,19 +27896,19 @@
     </row>
     <row r="600" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A600" s="12" t="s">
-        <v>163</v>
+        <v>624</v>
       </c>
       <c r="B600" s="12" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="C600" s="12" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="D600" s="12" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E600" s="12" t="s">
-        <v>4036</v>
+        <v>4035</v>
       </c>
       <c r="F600" s="12">
         <v>0</v>
@@ -27895,19 +27919,19 @@
     </row>
     <row r="601" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A601" s="12" t="s">
-        <v>435</v>
+        <v>163</v>
       </c>
       <c r="B601" s="12" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="C601" s="12" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="D601" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E601" s="12" t="s">
-        <v>4037</v>
+        <v>4036</v>
       </c>
       <c r="F601" s="12">
         <v>0</v>
@@ -27918,19 +27942,19 @@
     </row>
     <row r="602" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A602" s="12" t="s">
-        <v>177</v>
+        <v>435</v>
       </c>
       <c r="B602" s="12" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="C602" s="12" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="D602" s="12" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E602" s="12" t="s">
-        <v>4038</v>
+        <v>4037</v>
       </c>
       <c r="F602" s="12">
         <v>0</v>
@@ -27941,19 +27965,19 @@
     </row>
     <row r="603" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A603" s="12" t="s">
-        <v>455</v>
+        <v>177</v>
       </c>
       <c r="B603" s="12" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="C603" s="12" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="D603" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E603" s="12" t="s">
-        <v>4039</v>
+        <v>4038</v>
       </c>
       <c r="F603" s="12">
         <v>0</v>
@@ -27964,19 +27988,19 @@
     </row>
     <row r="604" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A604" s="12" t="s">
-        <v>147</v>
+        <v>455</v>
       </c>
       <c r="B604" s="12" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="C604" s="12" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="D604" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E604" s="12" t="s">
-        <v>4040</v>
+        <v>4039</v>
       </c>
       <c r="F604" s="12">
         <v>0</v>
@@ -27987,19 +28011,19 @@
     </row>
     <row r="605" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A605" s="12" t="s">
-        <v>627</v>
+        <v>147</v>
       </c>
       <c r="B605" s="12" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="C605" s="12" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D605" s="12" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E605" s="12" t="s">
-        <v>4041</v>
+        <v>4040</v>
       </c>
       <c r="F605" s="12">
         <v>0</v>
@@ -28010,62 +28034,62 @@
     </row>
     <row r="606" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A606" s="12" t="s">
-        <v>587</v>
+        <v>627</v>
       </c>
       <c r="B606" s="12" t="s">
-        <v>1078</v>
+        <v>1076</v>
+      </c>
+      <c r="C606" s="12" t="s">
+        <v>1077</v>
       </c>
       <c r="D606" s="12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E606" s="12" t="s">
-        <v>4042</v>
+        <v>4041</v>
       </c>
       <c r="F606" s="12">
         <v>0</v>
       </c>
       <c r="G606" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="607" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A607" s="12" t="s">
-        <v>164</v>
+        <v>587</v>
       </c>
       <c r="B607" s="12" t="s">
-        <v>1079</v>
-      </c>
-      <c r="C607" s="12" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="D607" s="12" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E607" s="12" t="s">
-        <v>4043</v>
+        <v>4042</v>
       </c>
       <c r="F607" s="12">
         <v>0</v>
       </c>
       <c r="G607" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="608" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A608" s="12" t="s">
-        <v>255</v>
+        <v>164</v>
       </c>
       <c r="B608" s="12" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="C608" s="12" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="D608" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E608" s="12" t="s">
-        <v>4044</v>
+        <v>4043</v>
       </c>
       <c r="F608" s="12">
         <v>0</v>
@@ -28076,19 +28100,19 @@
     </row>
     <row r="609" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A609" s="12" t="s">
-        <v>392</v>
+        <v>255</v>
       </c>
       <c r="B609" s="12" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="C609" s="12" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D609" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E609" s="12" t="s">
-        <v>4045</v>
+        <v>4044</v>
       </c>
       <c r="F609" s="12">
         <v>0</v>
@@ -28099,19 +28123,19 @@
     </row>
     <row r="610" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A610" s="12" t="s">
-        <v>245</v>
+        <v>392</v>
       </c>
       <c r="B610" s="12" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="C610" s="12" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="D610" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E610" s="12" t="s">
-        <v>4046</v>
+        <v>4045</v>
       </c>
       <c r="F610" s="12">
         <v>0</v>
@@ -28122,19 +28146,19 @@
     </row>
     <row r="611" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A611" s="12" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="B611" s="12" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="C611" s="12" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="D611" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E611" s="12" t="s">
-        <v>4047</v>
+        <v>4046</v>
       </c>
       <c r="F611" s="12">
         <v>0</v>
@@ -28145,19 +28169,19 @@
     </row>
     <row r="612" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A612" s="12" t="s">
-        <v>1291</v>
+        <v>220</v>
       </c>
       <c r="B612" s="12" t="s">
-        <v>1292</v>
+        <v>1087</v>
       </c>
       <c r="C612" s="12" t="s">
-        <v>1293</v>
+        <v>1088</v>
       </c>
       <c r="D612" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E612" s="12" t="s">
-        <v>4048</v>
+        <v>4047</v>
       </c>
       <c r="F612" s="12">
         <v>0</v>
@@ -28168,19 +28192,19 @@
     </row>
     <row r="613" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A613" s="12" t="s">
-        <v>190</v>
+        <v>1291</v>
       </c>
       <c r="B613" s="12" t="s">
-        <v>1089</v>
+        <v>1292</v>
       </c>
       <c r="C613" s="12" t="s">
-        <v>1090</v>
+        <v>1293</v>
       </c>
       <c r="D613" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E613" s="12" t="s">
-        <v>4049</v>
+        <v>4048</v>
       </c>
       <c r="F613" s="12">
         <v>0</v>
@@ -28191,16 +28215,19 @@
     </row>
     <row r="614" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A614" s="12" t="s">
-        <v>59</v>
+        <v>190</v>
       </c>
       <c r="B614" s="12" t="s">
-        <v>1091</v>
+        <v>1089</v>
+      </c>
+      <c r="C614" s="12" t="s">
+        <v>1090</v>
       </c>
       <c r="D614" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E614" s="12" t="s">
-        <v>4050</v>
+        <v>4049</v>
       </c>
       <c r="F614" s="12">
         <v>0</v>
@@ -28211,16 +28238,16 @@
     </row>
     <row r="615" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A615" s="12" t="s">
-        <v>193</v>
+        <v>59</v>
       </c>
       <c r="B615" s="12" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D615" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E615" s="12" t="s">
-        <v>4051</v>
+        <v>4050</v>
       </c>
       <c r="F615" s="12">
         <v>0</v>
@@ -28231,19 +28258,16 @@
     </row>
     <row r="616" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A616" s="12" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="B616" s="12" t="s">
-        <v>1093</v>
-      </c>
-      <c r="C616" s="12" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="D616" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E616" s="12" t="s">
-        <v>4052</v>
+        <v>4051</v>
       </c>
       <c r="F616" s="12">
         <v>0</v>
@@ -28254,19 +28278,19 @@
     </row>
     <row r="617" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A617" s="12" t="s">
-        <v>292</v>
+        <v>205</v>
       </c>
       <c r="B617" s="12" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="C617" s="12" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="D617" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E617" s="12" t="s">
-        <v>4053</v>
+        <v>4052</v>
       </c>
       <c r="F617" s="12">
         <v>0</v>
@@ -28277,19 +28301,19 @@
     </row>
     <row r="618" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A618" s="12" t="s">
-        <v>557</v>
+        <v>292</v>
       </c>
       <c r="B618" s="12" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="C618" s="12" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="D618" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E618" s="12" t="s">
-        <v>4054</v>
+        <v>4053</v>
       </c>
       <c r="F618" s="12">
         <v>0</v>
@@ -28300,19 +28324,19 @@
     </row>
     <row r="619" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A619" s="12" t="s">
-        <v>318</v>
+        <v>557</v>
       </c>
       <c r="B619" s="12" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="C619" s="12" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="D619" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E619" s="12" t="s">
-        <v>4055</v>
+        <v>4054</v>
       </c>
       <c r="F619" s="12">
         <v>0</v>
@@ -28323,16 +28347,19 @@
     </row>
     <row r="620" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A620" s="12" t="s">
-        <v>201</v>
+        <v>318</v>
       </c>
       <c r="B620" s="12" t="s">
-        <v>1101</v>
+        <v>1099</v>
+      </c>
+      <c r="C620" s="12" t="s">
+        <v>1100</v>
       </c>
       <c r="D620" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E620" s="12" t="s">
-        <v>4056</v>
+        <v>4055</v>
       </c>
       <c r="F620" s="12">
         <v>0</v>
@@ -28343,19 +28370,16 @@
     </row>
     <row r="621" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A621" s="12" t="s">
-        <v>497</v>
+        <v>201</v>
       </c>
       <c r="B621" s="12" t="s">
-        <v>1102</v>
-      </c>
-      <c r="C621" s="12" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="D621" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E621" s="12" t="s">
-        <v>4057</v>
+        <v>4056</v>
       </c>
       <c r="F621" s="12">
         <v>0</v>
@@ -28366,19 +28390,19 @@
     </row>
     <row r="622" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A622" s="12" t="s">
-        <v>559</v>
+        <v>497</v>
       </c>
       <c r="B622" s="12" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C622" s="12" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="D622" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E622" s="12" t="s">
-        <v>4058</v>
+        <v>4057</v>
       </c>
       <c r="F622" s="12">
         <v>0</v>
@@ -28389,19 +28413,19 @@
     </row>
     <row r="623" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A623" s="12" t="s">
-        <v>527</v>
+        <v>559</v>
       </c>
       <c r="B623" s="12" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C623" s="12" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="D623" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E623" s="12" t="s">
-        <v>4059</v>
+        <v>4058</v>
       </c>
       <c r="F623" s="12">
         <v>0</v>
@@ -28412,19 +28436,19 @@
     </row>
     <row r="624" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A624" s="12" t="s">
-        <v>293</v>
+        <v>527</v>
       </c>
       <c r="B624" s="12" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="C624" s="12" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="D624" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E624" s="12" t="s">
-        <v>4060</v>
+        <v>4059</v>
       </c>
       <c r="F624" s="12">
         <v>0</v>
@@ -28435,19 +28459,19 @@
     </row>
     <row r="625" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A625" s="12" t="s">
-        <v>447</v>
+        <v>293</v>
       </c>
       <c r="B625" s="12" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="C625" s="12" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="D625" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E625" s="12" t="s">
-        <v>4061</v>
+        <v>4060</v>
       </c>
       <c r="F625" s="12">
         <v>0</v>
@@ -28458,19 +28482,19 @@
     </row>
     <row r="626" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A626" s="12" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="B626" s="12" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C626" s="12" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="D626" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E626" s="12" t="s">
-        <v>4062</v>
+        <v>4061</v>
       </c>
       <c r="F626" s="12">
         <v>0</v>
@@ -28481,19 +28505,19 @@
     </row>
     <row r="627" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A627" s="12" t="s">
-        <v>333</v>
+        <v>460</v>
       </c>
       <c r="B627" s="12" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="C627" s="12" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="D627" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E627" s="12" t="s">
-        <v>4063</v>
+        <v>4062</v>
       </c>
       <c r="F627" s="12">
         <v>0</v>
@@ -28504,19 +28528,19 @@
     </row>
     <row r="628" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A628" s="12" t="s">
-        <v>428</v>
+        <v>333</v>
       </c>
       <c r="B628" s="12" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="C628" s="12" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="D628" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E628" s="12" t="s">
-        <v>4064</v>
+        <v>4063</v>
       </c>
       <c r="F628" s="12">
         <v>0</v>
@@ -28527,19 +28551,19 @@
     </row>
     <row r="629" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A629" s="12" t="s">
-        <v>537</v>
+        <v>428</v>
       </c>
       <c r="B629" s="12" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C629" s="12" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="D629" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E629" s="12" t="s">
-        <v>4065</v>
+        <v>4064</v>
       </c>
       <c r="F629" s="12">
         <v>0</v>
@@ -28550,19 +28574,19 @@
     </row>
     <row r="630" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A630" s="12" t="s">
-        <v>582</v>
+        <v>537</v>
       </c>
       <c r="B630" s="12" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="C630" s="12" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="D630" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E630" s="12" t="s">
-        <v>4066</v>
+        <v>4065</v>
       </c>
       <c r="F630" s="12">
         <v>0</v>
@@ -28573,19 +28597,19 @@
     </row>
     <row r="631" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A631" s="12" t="s">
-        <v>65</v>
+        <v>582</v>
       </c>
       <c r="B631" s="12" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="C631" s="12" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="D631" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E631" s="12" t="s">
-        <v>4067</v>
+        <v>4066</v>
       </c>
       <c r="F631" s="12">
         <v>0</v>
@@ -28596,19 +28620,19 @@
     </row>
     <row r="632" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A632" s="12" t="s">
-        <v>1294</v>
+        <v>65</v>
       </c>
       <c r="B632" s="12" t="s">
-        <v>1295</v>
+        <v>1122</v>
       </c>
       <c r="C632" s="12" t="s">
-        <v>1296</v>
+        <v>1123</v>
       </c>
       <c r="D632" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E632" s="12" t="s">
-        <v>4068</v>
+        <v>4067</v>
       </c>
       <c r="F632" s="12">
         <v>0</v>
@@ -28619,19 +28643,19 @@
     </row>
     <row r="633" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A633" s="12" t="s">
-        <v>1297</v>
+        <v>1294</v>
       </c>
       <c r="B633" s="12" t="s">
-        <v>1298</v>
+        <v>1295</v>
       </c>
       <c r="C633" s="12" t="s">
-        <v>1299</v>
+        <v>1296</v>
       </c>
       <c r="D633" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E633" s="12" t="s">
-        <v>4069</v>
+        <v>4068</v>
       </c>
       <c r="F633" s="12">
         <v>0</v>
@@ -28642,19 +28666,19 @@
     </row>
     <row r="634" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A634" s="12" t="s">
-        <v>99</v>
+        <v>1297</v>
       </c>
       <c r="B634" s="12" t="s">
-        <v>1124</v>
+        <v>1298</v>
       </c>
       <c r="C634" s="12" t="s">
-        <v>1125</v>
+        <v>1299</v>
       </c>
       <c r="D634" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E634" s="12" t="s">
-        <v>4070</v>
+        <v>4069</v>
       </c>
       <c r="F634" s="12">
         <v>0</v>
@@ -28665,19 +28689,19 @@
     </row>
     <row r="635" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A635" s="12" t="s">
-        <v>493</v>
+        <v>99</v>
       </c>
       <c r="B635" s="12" t="s">
-        <v>1300</v>
+        <v>1124</v>
       </c>
       <c r="C635" s="12" t="s">
-        <v>1301</v>
+        <v>1125</v>
       </c>
       <c r="D635" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E635" s="12" t="s">
-        <v>4071</v>
+        <v>4070</v>
       </c>
       <c r="F635" s="12">
         <v>0</v>
@@ -28688,19 +28712,19 @@
     </row>
     <row r="636" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A636" s="12" t="s">
-        <v>261</v>
+        <v>493</v>
       </c>
       <c r="B636" s="12" t="s">
-        <v>1126</v>
+        <v>1300</v>
       </c>
       <c r="C636" s="12" t="s">
-        <v>1127</v>
+        <v>1301</v>
       </c>
       <c r="D636" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E636" s="12" t="s">
-        <v>4072</v>
+        <v>4071</v>
       </c>
       <c r="F636" s="12">
         <v>0</v>
@@ -28710,20 +28734,20 @@
       </c>
     </row>
     <row r="637" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A637" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="B637" s="12" t="s">
-        <v>1128</v>
-      </c>
-      <c r="C637" s="12" t="s">
-        <v>1129</v>
+      <c r="A637" s="10" t="s">
+        <v>4300</v>
+      </c>
+      <c r="B637" s="10" t="s">
+        <v>4301</v>
+      </c>
+      <c r="C637" s="10" t="s">
+        <v>4302</v>
       </c>
       <c r="D637" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E637" s="12" t="s">
-        <v>4073</v>
+        <v>4303</v>
       </c>
       <c r="F637" s="12">
         <v>0</v>
@@ -28734,39 +28758,42 @@
     </row>
     <row r="638" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A638" s="12" t="s">
-        <v>457</v>
+        <v>261</v>
       </c>
       <c r="B638" s="12" t="s">
-        <v>1130</v>
+        <v>1126</v>
+      </c>
+      <c r="C638" s="12" t="s">
+        <v>1127</v>
       </c>
       <c r="D638" s="12" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E638" s="12" t="s">
-        <v>4074</v>
+        <v>4072</v>
       </c>
       <c r="F638" s="12">
         <v>0</v>
       </c>
       <c r="G638" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="639" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A639" s="12" t="s">
-        <v>681</v>
+        <v>332</v>
       </c>
       <c r="B639" s="12" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="C639" s="12" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="D639" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E639" s="12" t="s">
-        <v>4075</v>
+        <v>4073</v>
       </c>
       <c r="F639" s="12">
         <v>0</v>
@@ -28777,42 +28804,39 @@
     </row>
     <row r="640" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A640" s="12" t="s">
-        <v>4212</v>
+        <v>457</v>
       </c>
       <c r="B640" s="12" t="s">
-        <v>4168</v>
-      </c>
-      <c r="C640" s="12" t="s">
-        <v>4169</v>
+        <v>1130</v>
       </c>
       <c r="D640" s="12" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E640" s="12" t="s">
-        <v>4193</v>
+        <v>4074</v>
       </c>
       <c r="F640" s="12">
         <v>0</v>
       </c>
       <c r="G640" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="641" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A641" s="12" t="s">
-        <v>183</v>
+        <v>681</v>
       </c>
       <c r="B641" s="12" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="C641" s="12" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="D641" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E641" s="12" t="s">
-        <v>4076</v>
+        <v>4075</v>
       </c>
       <c r="F641" s="12">
         <v>0</v>
@@ -28823,19 +28847,19 @@
     </row>
     <row r="642" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A642" s="12" t="s">
-        <v>446</v>
+        <v>4212</v>
       </c>
       <c r="B642" s="12" t="s">
-        <v>1135</v>
+        <v>4168</v>
       </c>
       <c r="C642" s="12" t="s">
-        <v>1136</v>
+        <v>4169</v>
       </c>
       <c r="D642" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E642" s="12" t="s">
-        <v>4077</v>
+        <v>4193</v>
       </c>
       <c r="F642" s="12">
         <v>0</v>
@@ -28846,19 +28870,19 @@
     </row>
     <row r="643" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A643" s="12" t="s">
-        <v>697</v>
+        <v>183</v>
       </c>
       <c r="B643" s="12" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="C643" s="12" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="D643" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E643" s="12" t="s">
-        <v>4078</v>
+        <v>4076</v>
       </c>
       <c r="F643" s="12">
         <v>0</v>
@@ -28869,19 +28893,19 @@
     </row>
     <row r="644" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A644" s="12" t="s">
-        <v>685</v>
+        <v>446</v>
       </c>
       <c r="B644" s="12" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="C644" s="12" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="D644" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E644" s="12" t="s">
-        <v>4079</v>
+        <v>4077</v>
       </c>
       <c r="F644" s="12">
         <v>0</v>
@@ -28892,19 +28916,19 @@
     </row>
     <row r="645" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A645" s="12" t="s">
-        <v>673</v>
+        <v>697</v>
       </c>
       <c r="B645" s="12" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="C645" s="12" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="D645" s="12" t="s">
         <v>43</v>
       </c>
       <c r="E645" s="12" t="s">
-        <v>4080</v>
+        <v>4078</v>
       </c>
       <c r="F645" s="12">
         <v>0</v>
@@ -28915,19 +28939,19 @@
     </row>
     <row r="646" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A646" s="12" t="s">
-        <v>670</v>
+        <v>685</v>
       </c>
       <c r="B646" s="12" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="C646" s="12" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="D646" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E646" s="12" t="s">
-        <v>4081</v>
+        <v>4079</v>
       </c>
       <c r="F646" s="12">
         <v>0</v>
@@ -28938,19 +28962,19 @@
     </row>
     <row r="647" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A647" s="12" t="s">
-        <v>256</v>
+        <v>673</v>
       </c>
       <c r="B647" s="12" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="C647" s="12" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="D647" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E647" s="12" t="s">
-        <v>4082</v>
+        <v>4080</v>
       </c>
       <c r="F647" s="12">
         <v>0</v>
@@ -28961,19 +28985,19 @@
     </row>
     <row r="648" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A648" s="12" t="s">
-        <v>267</v>
+        <v>670</v>
       </c>
       <c r="B648" s="12" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="C648" s="12" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="D648" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E648" s="12" t="s">
-        <v>4083</v>
+        <v>4081</v>
       </c>
       <c r="F648" s="12">
         <v>0</v>
@@ -28984,19 +29008,19 @@
     </row>
     <row r="649" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A649" s="12" t="s">
-        <v>575</v>
+        <v>256</v>
       </c>
       <c r="B649" s="12" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="C649" s="12" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="D649" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E649" s="12" t="s">
-        <v>4084</v>
+        <v>4082</v>
       </c>
       <c r="F649" s="12">
         <v>0</v>
@@ -29007,19 +29031,19 @@
     </row>
     <row r="650" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A650" s="12" t="s">
-        <v>538</v>
+        <v>267</v>
       </c>
       <c r="B650" s="12" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="C650" s="12" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="D650" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E650" s="12" t="s">
-        <v>4085</v>
+        <v>4083</v>
       </c>
       <c r="F650" s="12">
         <v>0</v>
@@ -29030,19 +29054,19 @@
     </row>
     <row r="651" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A651" s="12" t="s">
-        <v>370</v>
+        <v>575</v>
       </c>
       <c r="B651" s="12" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="C651" s="12" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="D651" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E651" s="12" t="s">
-        <v>4086</v>
+        <v>4084</v>
       </c>
       <c r="F651" s="12">
         <v>0</v>
@@ -29053,19 +29077,19 @@
     </row>
     <row r="652" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A652" s="12" t="s">
-        <v>334</v>
+        <v>538</v>
       </c>
       <c r="B652" s="12" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="C652" s="12" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="D652" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E652" s="12" t="s">
-        <v>4087</v>
+        <v>4085</v>
       </c>
       <c r="F652" s="12">
         <v>0</v>
@@ -29076,19 +29100,19 @@
     </row>
     <row r="653" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A653" s="12" t="s">
-        <v>613</v>
+        <v>370</v>
       </c>
       <c r="B653" s="12" t="s">
-        <v>1302</v>
+        <v>1153</v>
       </c>
       <c r="C653" s="12" t="s">
-        <v>1303</v>
+        <v>1154</v>
       </c>
       <c r="D653" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E653" s="12" t="s">
-        <v>4088</v>
+        <v>4086</v>
       </c>
       <c r="F653" s="12">
         <v>0</v>
@@ -29099,19 +29123,19 @@
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A654" s="12" t="s">
-        <v>102</v>
+        <v>334</v>
       </c>
       <c r="B654" s="12" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="C654" s="12" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="D654" s="12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E654" s="12" t="s">
-        <v>4089</v>
+        <v>4087</v>
       </c>
       <c r="F654" s="12">
         <v>0</v>
@@ -29122,19 +29146,19 @@
     </row>
     <row r="655" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A655" s="12" t="s">
-        <v>466</v>
+        <v>613</v>
       </c>
       <c r="B655" s="12" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="C655" s="12" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="D655" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E655" s="12" t="s">
-        <v>4090</v>
+        <v>4088</v>
       </c>
       <c r="F655" s="12">
         <v>0</v>
@@ -29145,19 +29169,19 @@
     </row>
     <row r="656" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A656" s="12" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B656" s="12" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="C656" s="12" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="D656" s="12" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E656" s="12" t="s">
-        <v>4091</v>
+        <v>4089</v>
       </c>
       <c r="F656" s="12">
         <v>0</v>
@@ -29168,19 +29192,19 @@
     </row>
     <row r="657" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A657" s="12" t="s">
-        <v>105</v>
+        <v>466</v>
       </c>
       <c r="B657" s="12" t="s">
-        <v>1161</v>
+        <v>1304</v>
       </c>
       <c r="C657" s="12" t="s">
-        <v>1162</v>
+        <v>1305</v>
       </c>
       <c r="D657" s="12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E657" s="12" t="s">
-        <v>4092</v>
+        <v>4090</v>
       </c>
       <c r="F657" s="12">
         <v>0</v>
@@ -29191,19 +29215,19 @@
     </row>
     <row r="658" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A658" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B658" s="12" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="C658" s="12" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
       <c r="D658" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E658" s="12" t="s">
-        <v>4093</v>
+        <v>4091</v>
       </c>
       <c r="F658" s="12">
         <v>0</v>
@@ -29214,19 +29238,19 @@
     </row>
     <row r="659" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A659" s="12" t="s">
-        <v>477</v>
+        <v>105</v>
       </c>
       <c r="B659" s="12" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
       <c r="C659" s="12" t="s">
-        <v>1166</v>
+        <v>1162</v>
       </c>
       <c r="D659" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E659" s="12" t="s">
-        <v>4094</v>
+        <v>4092</v>
       </c>
       <c r="F659" s="12">
         <v>0</v>
@@ -29237,19 +29261,19 @@
     </row>
     <row r="660" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A660" s="12" t="s">
-        <v>216</v>
+        <v>110</v>
       </c>
       <c r="B660" s="12" t="s">
-        <v>1167</v>
+        <v>1163</v>
       </c>
       <c r="C660" s="12" t="s">
-        <v>1168</v>
+        <v>1164</v>
       </c>
       <c r="D660" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E660" s="12" t="s">
-        <v>4095</v>
+        <v>4093</v>
       </c>
       <c r="F660" s="12">
         <v>0</v>
@@ -29260,19 +29284,19 @@
     </row>
     <row r="661" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A661" s="12" t="s">
-        <v>188</v>
+        <v>477</v>
       </c>
       <c r="B661" s="12" t="s">
-        <v>1169</v>
+        <v>1165</v>
       </c>
       <c r="C661" s="12" t="s">
-        <v>1170</v>
+        <v>1166</v>
       </c>
       <c r="D661" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E661" s="12" t="s">
-        <v>4096</v>
+        <v>4094</v>
       </c>
       <c r="F661" s="12">
         <v>0</v>
@@ -29283,19 +29307,19 @@
     </row>
     <row r="662" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A662" s="12" t="s">
-        <v>130</v>
+        <v>216</v>
       </c>
       <c r="B662" s="12" t="s">
-        <v>1171</v>
+        <v>1167</v>
       </c>
       <c r="C662" s="12" t="s">
-        <v>1172</v>
+        <v>1168</v>
       </c>
       <c r="D662" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E662" s="12" t="s">
-        <v>4097</v>
+        <v>4095</v>
       </c>
       <c r="F662" s="12">
         <v>0</v>
@@ -29306,19 +29330,19 @@
     </row>
     <row r="663" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A663" s="12" t="s">
-        <v>476</v>
+        <v>188</v>
       </c>
       <c r="B663" s="12" t="s">
-        <v>1173</v>
+        <v>1169</v>
       </c>
       <c r="C663" s="12" t="s">
-        <v>1174</v>
+        <v>1170</v>
       </c>
       <c r="D663" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E663" s="12" t="s">
-        <v>4098</v>
+        <v>4096</v>
       </c>
       <c r="F663" s="12">
         <v>0</v>
@@ -29329,19 +29353,19 @@
     </row>
     <row r="664" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A664" s="12" t="s">
-        <v>360</v>
+        <v>130</v>
       </c>
       <c r="B664" s="12" t="s">
-        <v>1175</v>
+        <v>1171</v>
       </c>
       <c r="C664" s="12" t="s">
-        <v>1176</v>
+        <v>1172</v>
       </c>
       <c r="D664" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E664" s="12" t="s">
-        <v>4099</v>
+        <v>4097</v>
       </c>
       <c r="F664" s="12">
         <v>0</v>
@@ -29352,19 +29376,19 @@
     </row>
     <row r="665" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A665" s="12" t="s">
-        <v>666</v>
+        <v>476</v>
       </c>
       <c r="B665" s="12" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="C665" s="12" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="D665" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E665" s="12" t="s">
-        <v>4100</v>
+        <v>4098</v>
       </c>
       <c r="F665" s="12">
         <v>0</v>
@@ -29375,19 +29399,19 @@
     </row>
     <row r="666" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A666" s="12" t="s">
-        <v>4213</v>
+        <v>360</v>
       </c>
       <c r="B666" s="12" t="s">
-        <v>4170</v>
+        <v>1175</v>
       </c>
       <c r="C666" s="12" t="s">
-        <v>4171</v>
+        <v>1176</v>
       </c>
       <c r="D666" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E666" s="12" t="s">
-        <v>4194</v>
+        <v>4099</v>
       </c>
       <c r="F666" s="12">
         <v>0</v>
@@ -29398,19 +29422,19 @@
     </row>
     <row r="667" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A667" s="12" t="s">
-        <v>1326</v>
+        <v>666</v>
       </c>
       <c r="B667" s="12" t="s">
-        <v>1327</v>
+        <v>1177</v>
       </c>
       <c r="C667" s="12" t="s">
-        <v>1328</v>
+        <v>1178</v>
       </c>
       <c r="D667" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E667" s="12" t="s">
-        <v>4101</v>
+        <v>4100</v>
       </c>
       <c r="F667" s="12">
         <v>0</v>
@@ -29421,19 +29445,19 @@
     </row>
     <row r="668" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A668" s="12" t="s">
-        <v>4214</v>
+        <v>4213</v>
       </c>
       <c r="B668" s="12" t="s">
-        <v>4172</v>
+        <v>4170</v>
       </c>
       <c r="C668" s="12" t="s">
-        <v>4173</v>
+        <v>4171</v>
       </c>
       <c r="D668" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E668" s="12" t="s">
-        <v>4195</v>
+        <v>4194</v>
       </c>
       <c r="F668" s="12">
         <v>0</v>
@@ -29444,19 +29468,19 @@
     </row>
     <row r="669" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A669" s="12" t="s">
-        <v>4215</v>
+        <v>1326</v>
       </c>
       <c r="B669" s="12" t="s">
-        <v>4174</v>
+        <v>1327</v>
       </c>
       <c r="C669" s="12" t="s">
-        <v>4175</v>
+        <v>1328</v>
       </c>
       <c r="D669" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E669" s="12" t="s">
-        <v>4196</v>
+        <v>4101</v>
       </c>
       <c r="F669" s="12">
         <v>0</v>
@@ -29467,19 +29491,19 @@
     </row>
     <row r="670" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A670" s="12" t="s">
-        <v>273</v>
+        <v>4214</v>
       </c>
       <c r="B670" s="12" t="s">
-        <v>1179</v>
+        <v>4172</v>
       </c>
       <c r="C670" s="12" t="s">
-        <v>1180</v>
+        <v>4173</v>
       </c>
       <c r="D670" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E670" s="12" t="s">
-        <v>4102</v>
+        <v>4195</v>
       </c>
       <c r="F670" s="12">
         <v>0</v>
@@ -29490,19 +29514,19 @@
     </row>
     <row r="671" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A671" s="12" t="s">
-        <v>660</v>
+        <v>4215</v>
       </c>
       <c r="B671" s="12" t="s">
-        <v>1181</v>
+        <v>4174</v>
       </c>
       <c r="C671" s="12" t="s">
-        <v>1182</v>
+        <v>4175</v>
       </c>
       <c r="D671" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E671" s="12" t="s">
-        <v>4103</v>
+        <v>4196</v>
       </c>
       <c r="F671" s="12">
         <v>0</v>
@@ -29513,19 +29537,19 @@
     </row>
     <row r="672" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A672" s="12" t="s">
-        <v>95</v>
+        <v>273</v>
       </c>
       <c r="B672" s="12" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="C672" s="12" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="D672" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E672" s="12" t="s">
-        <v>4104</v>
+        <v>4102</v>
       </c>
       <c r="F672" s="12">
         <v>0</v>
@@ -29536,19 +29560,19 @@
     </row>
     <row r="673" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A673" s="12" t="s">
-        <v>418</v>
+        <v>660</v>
       </c>
       <c r="B673" s="12" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="C673" s="12" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="D673" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E673" s="12" t="s">
-        <v>4105</v>
+        <v>4103</v>
       </c>
       <c r="F673" s="12">
         <v>0</v>
@@ -29559,19 +29583,19 @@
     </row>
     <row r="674" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A674" s="12" t="s">
-        <v>380</v>
+        <v>95</v>
       </c>
       <c r="B674" s="12" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="C674" s="12" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="D674" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E674" s="12" t="s">
-        <v>4106</v>
+        <v>4104</v>
       </c>
       <c r="F674" s="12">
         <v>0</v>
@@ -29582,19 +29606,19 @@
     </row>
     <row r="675" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A675" s="12" t="s">
-        <v>593</v>
+        <v>418</v>
       </c>
       <c r="B675" s="12" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="C675" s="12" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="D675" s="12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E675" s="12" t="s">
-        <v>4107</v>
+        <v>4105</v>
       </c>
       <c r="F675" s="12">
         <v>0</v>
@@ -29605,16 +29629,19 @@
     </row>
     <row r="676" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A676" s="12" t="s">
-        <v>231</v>
+        <v>380</v>
       </c>
       <c r="B676" s="12" t="s">
-        <v>1191</v>
+        <v>1187</v>
+      </c>
+      <c r="C676" s="12" t="s">
+        <v>1188</v>
       </c>
       <c r="D676" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E676" s="12" t="s">
-        <v>4108</v>
+        <v>4106</v>
       </c>
       <c r="F676" s="12">
         <v>0</v>
@@ -29625,19 +29652,19 @@
     </row>
     <row r="677" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A677" s="12" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="B677" s="12" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
       <c r="C677" s="12" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
       <c r="D677" s="12" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E677" s="12" t="s">
-        <v>4109</v>
+        <v>4107</v>
       </c>
       <c r="F677" s="12">
         <v>0</v>
@@ -29648,19 +29675,16 @@
     </row>
     <row r="678" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A678" s="12" t="s">
-        <v>184</v>
+        <v>231</v>
       </c>
       <c r="B678" s="12" t="s">
-        <v>1194</v>
-      </c>
-      <c r="C678" s="12" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="D678" s="12" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E678" s="12" t="s">
-        <v>4110</v>
+        <v>4108</v>
       </c>
       <c r="F678" s="12">
         <v>0</v>
@@ -29671,19 +29695,19 @@
     </row>
     <row r="679" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A679" s="12" t="s">
-        <v>329</v>
+        <v>606</v>
       </c>
       <c r="B679" s="12" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="C679" s="12" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="D679" s="12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E679" s="12" t="s">
-        <v>4111</v>
+        <v>4109</v>
       </c>
       <c r="F679" s="12">
         <v>0</v>
@@ -29694,19 +29718,19 @@
     </row>
     <row r="680" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A680" s="12" t="s">
-        <v>478</v>
+        <v>184</v>
       </c>
       <c r="B680" s="12" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="C680" s="12" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="D680" s="12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E680" s="12" t="s">
-        <v>4112</v>
+        <v>4110</v>
       </c>
       <c r="F680" s="12">
         <v>0</v>
@@ -29717,19 +29741,19 @@
     </row>
     <row r="681" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A681" s="12" t="s">
-        <v>689</v>
+        <v>329</v>
       </c>
       <c r="B681" s="12" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="C681" s="12" t="s">
-        <v>1190</v>
+        <v>1197</v>
       </c>
       <c r="D681" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E681" s="12" t="s">
-        <v>4113</v>
+        <v>4111</v>
       </c>
       <c r="F681" s="12">
         <v>0</v>
@@ -29740,19 +29764,19 @@
     </row>
     <row r="682" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A682" s="12" t="s">
-        <v>104</v>
+        <v>478</v>
       </c>
       <c r="B682" s="12" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="C682" s="12" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
       <c r="D682" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E682" s="12" t="s">
-        <v>4114</v>
+        <v>4112</v>
       </c>
       <c r="F682" s="12">
         <v>0</v>
@@ -29763,19 +29787,19 @@
     </row>
     <row r="683" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A683" s="12" t="s">
-        <v>636</v>
+        <v>689</v>
       </c>
       <c r="B683" s="12" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="C683" s="12" t="s">
-        <v>1204</v>
+        <v>1190</v>
       </c>
       <c r="D683" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E683" s="12" t="s">
-        <v>4115</v>
+        <v>4113</v>
       </c>
       <c r="F683" s="12">
         <v>0</v>
@@ -29786,19 +29810,19 @@
     </row>
     <row r="684" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A684" s="12" t="s">
-        <v>621</v>
+        <v>104</v>
       </c>
       <c r="B684" s="12" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="C684" s="12" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="D684" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E684" s="12" t="s">
-        <v>4116</v>
+        <v>4114</v>
       </c>
       <c r="F684" s="12">
         <v>0</v>
@@ -29809,19 +29833,19 @@
     </row>
     <row r="685" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A685" s="12" t="s">
-        <v>120</v>
+        <v>636</v>
       </c>
       <c r="B685" s="12" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="C685" s="12" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="D685" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E685" s="12" t="s">
-        <v>4117</v>
+        <v>4115</v>
       </c>
       <c r="F685" s="12">
         <v>0</v>
@@ -29832,19 +29856,19 @@
     </row>
     <row r="686" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A686" s="12" t="s">
-        <v>154</v>
+        <v>621</v>
       </c>
       <c r="B686" s="12" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="C686" s="12" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="D686" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E686" s="12" t="s">
-        <v>4118</v>
+        <v>4116</v>
       </c>
       <c r="F686" s="12">
         <v>0</v>
@@ -29855,16 +29879,19 @@
     </row>
     <row r="687" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A687" s="12" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B687" s="12" t="s">
-        <v>1211</v>
+        <v>1207</v>
+      </c>
+      <c r="C687" s="12" t="s">
+        <v>1208</v>
       </c>
       <c r="D687" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E687" s="12" t="s">
-        <v>4119</v>
+        <v>4117</v>
       </c>
       <c r="F687" s="12">
         <v>0</v>
@@ -29875,19 +29902,19 @@
     </row>
     <row r="688" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A688" s="12" t="s">
-        <v>269</v>
+        <v>154</v>
       </c>
       <c r="B688" s="12" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="C688" s="12" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="D688" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E688" s="12" t="s">
-        <v>4120</v>
+        <v>4118</v>
       </c>
       <c r="F688" s="12">
         <v>0</v>
@@ -29898,19 +29925,16 @@
     </row>
     <row r="689" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A689" s="12" t="s">
-        <v>607</v>
+        <v>137</v>
       </c>
       <c r="B689" s="12" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C689" s="12" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="D689" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E689" s="12" t="s">
-        <v>4121</v>
+        <v>4119</v>
       </c>
       <c r="F689" s="12">
         <v>0</v>
@@ -29921,19 +29945,19 @@
     </row>
     <row r="690" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A690" s="12" t="s">
-        <v>402</v>
+        <v>269</v>
       </c>
       <c r="B690" s="12" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="C690" s="12" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="D690" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E690" s="12" t="s">
-        <v>4122</v>
+        <v>4120</v>
       </c>
       <c r="F690" s="12">
         <v>0</v>
@@ -29944,19 +29968,19 @@
     </row>
     <row r="691" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A691" s="12" t="s">
-        <v>399</v>
+        <v>607</v>
       </c>
       <c r="B691" s="12" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="C691" s="12" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="D691" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E691" s="12" t="s">
-        <v>4123</v>
+        <v>4121</v>
       </c>
       <c r="F691" s="12">
         <v>0</v>
@@ -29967,19 +29991,19 @@
     </row>
     <row r="692" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A692" s="12" t="s">
-        <v>452</v>
+        <v>402</v>
       </c>
       <c r="B692" s="12" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="C692" s="12" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="D692" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E692" s="12" t="s">
-        <v>4124</v>
+        <v>4122</v>
       </c>
       <c r="F692" s="12">
         <v>0</v>
@@ -29990,19 +30014,19 @@
     </row>
     <row r="693" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A693" s="12" t="s">
-        <v>107</v>
+        <v>399</v>
       </c>
       <c r="B693" s="12" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="C693" s="12" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="D693" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E693" s="12" t="s">
-        <v>4125</v>
+        <v>4123</v>
       </c>
       <c r="F693" s="12">
         <v>0</v>
@@ -30013,16 +30037,19 @@
     </row>
     <row r="694" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A694" s="12" t="s">
-        <v>114</v>
+        <v>452</v>
       </c>
       <c r="B694" s="12" t="s">
-        <v>1224</v>
+        <v>1220</v>
+      </c>
+      <c r="C694" s="12" t="s">
+        <v>1221</v>
       </c>
       <c r="D694" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E694" s="12" t="s">
-        <v>4126</v>
+        <v>4124</v>
       </c>
       <c r="F694" s="12">
         <v>0</v>
@@ -30033,19 +30060,19 @@
     </row>
     <row r="695" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A695" s="12" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B695" s="12" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="C695" s="12" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="D695" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E695" s="12" t="s">
-        <v>4127</v>
+        <v>4125</v>
       </c>
       <c r="F695" s="12">
         <v>0</v>
@@ -30056,19 +30083,16 @@
     </row>
     <row r="696" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A696" s="12" t="s">
-        <v>554</v>
+        <v>114</v>
       </c>
       <c r="B696" s="12" t="s">
-        <v>1227</v>
-      </c>
-      <c r="C696" s="12" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="D696" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E696" s="12" t="s">
-        <v>4128</v>
+        <v>4126</v>
       </c>
       <c r="F696" s="12">
         <v>0</v>
@@ -30079,19 +30103,19 @@
     </row>
     <row r="697" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A697" s="12" t="s">
-        <v>192</v>
+        <v>118</v>
       </c>
       <c r="B697" s="12" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="C697" s="12" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="D697" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E697" s="12" t="s">
-        <v>4129</v>
+        <v>4127</v>
       </c>
       <c r="F697" s="12">
         <v>0</v>
@@ -30102,16 +30126,19 @@
     </row>
     <row r="698" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A698" s="12" t="s">
-        <v>278</v>
+        <v>554</v>
       </c>
       <c r="B698" s="12" t="s">
-        <v>1231</v>
+        <v>1227</v>
+      </c>
+      <c r="C698" s="12" t="s">
+        <v>1228</v>
       </c>
       <c r="D698" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E698" s="12" t="s">
-        <v>4130</v>
+        <v>4128</v>
       </c>
       <c r="F698" s="12">
         <v>0</v>
@@ -30122,19 +30149,19 @@
     </row>
     <row r="699" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A699" s="12" t="s">
-        <v>309</v>
+        <v>192</v>
       </c>
       <c r="B699" s="12" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="C699" s="12" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="D699" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E699" s="12" t="s">
-        <v>4131</v>
+        <v>4129</v>
       </c>
       <c r="F699" s="12">
         <v>0</v>
@@ -30145,19 +30172,16 @@
     </row>
     <row r="700" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A700" s="12" t="s">
-        <v>64</v>
+        <v>278</v>
       </c>
       <c r="B700" s="12" t="s">
-        <v>1234</v>
-      </c>
-      <c r="C700" s="12" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="D700" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E700" s="12" t="s">
-        <v>4132</v>
+        <v>4130</v>
       </c>
       <c r="F700" s="12">
         <v>0</v>
@@ -30168,19 +30192,19 @@
     </row>
     <row r="701" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A701" s="12" t="s">
-        <v>481</v>
+        <v>309</v>
       </c>
       <c r="B701" s="12" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
       <c r="C701" s="12" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="D701" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E701" s="12" t="s">
-        <v>4133</v>
+        <v>4131</v>
       </c>
       <c r="F701" s="12">
         <v>0</v>
@@ -30191,39 +30215,42 @@
     </row>
     <row r="702" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A702" s="12" t="s">
-        <v>550</v>
+        <v>64</v>
       </c>
       <c r="B702" s="12" t="s">
-        <v>1238</v>
+        <v>1234</v>
+      </c>
+      <c r="C702" s="12" t="s">
+        <v>1235</v>
       </c>
       <c r="D702" s="12" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E702" s="12" t="s">
-        <v>4134</v>
+        <v>4132</v>
       </c>
       <c r="F702" s="12">
         <v>0</v>
       </c>
       <c r="G702" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="703" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A703" s="12" t="s">
-        <v>618</v>
+        <v>481</v>
       </c>
       <c r="B703" s="12" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="C703" s="12" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="D703" s="12" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E703" s="12" t="s">
-        <v>4135</v>
+        <v>4133</v>
       </c>
       <c r="F703" s="12">
         <v>0</v>
@@ -30234,54 +30261,97 @@
     </row>
     <row r="704" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A704" s="12" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
       <c r="B704" s="12" t="s">
-        <v>1241</v>
-      </c>
-      <c r="C704" s="12" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="D704" s="12" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="E704" s="12" t="s">
-        <v>4136</v>
+        <v>4134</v>
       </c>
       <c r="F704" s="12">
         <v>0</v>
       </c>
       <c r="G704" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="705" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A705" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="B705" s="12" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C705" s="12" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D705" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E705" s="12" t="s">
+        <v>4135</v>
+      </c>
+      <c r="F705" s="12">
+        <v>0</v>
+      </c>
+      <c r="G705" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="706" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A706" s="12" t="s">
+        <v>563</v>
+      </c>
+      <c r="B706" s="12" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C706" s="12" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D706" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E706" s="12" t="s">
+        <v>4136</v>
+      </c>
+      <c r="F706" s="12">
+        <v>0</v>
+      </c>
+      <c r="G706" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="707" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A707" s="12" t="s">
         <v>424</v>
       </c>
-      <c r="B705" s="12" t="s">
+      <c r="B707" s="12" t="s">
         <v>1243</v>
       </c>
-      <c r="C705" s="12" t="s">
+      <c r="C707" s="12" t="s">
         <v>1244</v>
       </c>
-      <c r="D705" s="12" t="s">
+      <c r="D707" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E705" s="12" t="s">
+      <c r="E707" s="12" t="s">
         <v>4137</v>
       </c>
-      <c r="F705" s="12">
-        <v>0</v>
-      </c>
-      <c r="G705" s="12">
+      <c r="F707" s="12">
+        <v>0</v>
+      </c>
+      <c r="G707" s="12">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G705">
-    <sortState ref="A2:G706">
-      <sortCondition ref="A1:A706"/>
+  <autoFilter ref="A1:G707">
+    <sortState ref="A2:G707">
+      <sortCondition ref="A1:A707"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Further tweaks to error checking and removed hardcoded path
</commit_message>
<xml_diff>
--- a/GazetteerETL/Resources/UniversalGazetterModel.xlsx
+++ b/GazetteerETL/Resources/UniversalGazetterModel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7643" uniqueCount="4314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7648" uniqueCount="4318">
   <si>
     <t>RECORD_ID</t>
   </si>
@@ -12969,6 +12969,18 @@
   </si>
   <si>
     <t>A-ADM5</t>
+  </si>
+  <si>
+    <t>INSTALLATION</t>
+  </si>
+  <si>
+    <t>generic installation</t>
+  </si>
+  <si>
+    <t>a generic installation for use when a source does not provide more specific type</t>
+  </si>
+  <si>
+    <t>S-INSTALLATION</t>
   </si>
 </sst>
 </file>
@@ -14307,17 +14319,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G708"/>
+  <dimension ref="A1:G709"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A673" workbookViewId="0">
+      <selection activeCell="F710" sqref="F710"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="47.85546875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="72.5703125" style="12" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.28515625" style="12" bestFit="1" customWidth="1"/>
@@ -30420,6 +30432,29 @@
         <v>0</v>
       </c>
       <c r="G708" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="709" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A709" s="12" t="s">
+        <v>4314</v>
+      </c>
+      <c r="B709" s="12" t="s">
+        <v>4315</v>
+      </c>
+      <c r="C709" s="12" t="s">
+        <v>4316</v>
+      </c>
+      <c r="D709" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E709" s="12" t="s">
+        <v>4317</v>
+      </c>
+      <c r="F709" s="12">
+        <v>0</v>
+      </c>
+      <c r="G709" s="12">
         <v>0</v>
       </c>
     </row>

</xml_diff>